<commit_message>
verifying regfile, checking sta segmentation fault
</commit_message>
<xml_diff>
--- a/dynamic_power_analysis/code/OpenSTA_report_power/dynamic_power_analysis.xlsx
+++ b/dynamic_power_analysis/code/OpenSTA_report_power/dynamic_power_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/youssef/Desktop/EDA/Dynamic_Power_Clock_Gating/dynamic_power_analysis/code/OpenSTA_report_power/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB75F77-34F1-F240-A737-534CA6602689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0198BFB5-69A9-0748-9CFF-ED3D4C1D3B0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14160" xr2:uid="{42F2CD03-9D47-9445-8059-7D7C13E91239}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{42F2CD03-9D47-9445-8059-7D7C13E91239}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t xml:space="preserve">module </t>
   </si>
@@ -102,13 +102,31 @@
   </si>
   <si>
     <t>riscv</t>
+  </si>
+  <si>
+    <t>https://github.com/The-OpenROAD-Project/OpenLane/tree/master/regression_results</t>
+  </si>
+  <si>
+    <t>y_dct</t>
+  </si>
+  <si>
+    <t>ldpc_decoder_802_3an</t>
+  </si>
+  <si>
+    <t>chacha</t>
+  </si>
+  <si>
+    <t>ldpcenc</t>
+  </si>
+  <si>
+    <t>]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -176,6 +194,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -215,7 +253,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="36">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -461,19 +499,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -676,12 +701,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -689,23 +765,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="2" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="2" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -713,7 +783,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -722,7 +792,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="2" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="2" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -730,11 +800,11 @@
     <xf numFmtId="11" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="6" fillId="4" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="6" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="6" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="6" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -743,13 +813,26 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -759,21 +842,21 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="11" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="11" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="11" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1087,15 +1170,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3E8C89-AABD-1C41-B99B-18B443C74BC8}">
-  <dimension ref="D6:U20"/>
+  <dimension ref="D6:Z52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="63" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="64" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="T34" sqref="T34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" customWidth="1"/>
     <col min="5" max="5" width="30.33203125" customWidth="1"/>
     <col min="6" max="6" width="20.6640625" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
@@ -1106,7 +1189,7 @@
     <col min="13" max="13" width="20.33203125" customWidth="1"/>
     <col min="14" max="14" width="19" customWidth="1"/>
     <col min="15" max="15" width="17.1640625" customWidth="1"/>
-    <col min="16" max="16" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.6640625" customWidth="1"/>
     <col min="17" max="17" width="24.33203125" customWidth="1"/>
     <col min="18" max="18" width="15" customWidth="1"/>
     <col min="19" max="19" width="13.5" customWidth="1"/>
@@ -1134,168 +1217,168 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="56" t="s">
+      <c r="H7" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="57"/>
-      <c r="J7" s="57"/>
-      <c r="K7" s="57"/>
-      <c r="L7" s="49"/>
-      <c r="M7" s="57" t="s">
+      <c r="I7" s="66"/>
+      <c r="J7" s="66"/>
+      <c r="K7" s="66"/>
+      <c r="L7" s="45"/>
+      <c r="M7" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="N7" s="57"/>
-      <c r="O7" s="57"/>
-      <c r="P7" s="58"/>
-      <c r="Q7" s="50"/>
-      <c r="R7" s="57" t="s">
+      <c r="N7" s="66"/>
+      <c r="O7" s="66"/>
+      <c r="P7" s="67"/>
+      <c r="Q7" s="46"/>
+      <c r="R7" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="S7" s="57"/>
-      <c r="T7" s="57"/>
-      <c r="U7" s="58"/>
+      <c r="S7" s="66"/>
+      <c r="T7" s="66"/>
+      <c r="U7" s="67"/>
     </row>
     <row r="8" spans="4:21" ht="25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D8" s="55" t="s">
+      <c r="D8" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="53" t="s">
+      <c r="E8" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="F8" s="44" t="s">
+      <c r="F8" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="54" t="s">
+      <c r="G8" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="42" t="s">
+      <c r="H8" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="43" t="s">
+      <c r="I8" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="J8" s="44" t="s">
+      <c r="J8" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="45" t="s">
+      <c r="K8" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="L8" s="46"/>
-      <c r="M8" s="43" t="s">
+      <c r="L8" s="42"/>
+      <c r="M8" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="N8" s="43" t="s">
+      <c r="N8" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="O8" s="45" t="s">
+      <c r="O8" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="P8" s="47" t="s">
+      <c r="P8" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="Q8" s="48"/>
-      <c r="R8" s="43" t="s">
+      <c r="Q8" s="44"/>
+      <c r="R8" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="S8" s="42" t="s">
+      <c r="S8" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="T8" s="45" t="s">
+      <c r="T8" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="U8" s="47" t="s">
+      <c r="U8" s="43" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="4:21" ht="24" x14ac:dyDescent="0.3">
-      <c r="D9" s="59" t="s">
+      <c r="D9" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="60">
+      <c r="E9" s="53">
         <v>513</v>
       </c>
-      <c r="F9" s="61">
+      <c r="F9" s="54">
         <v>55531</v>
       </c>
-      <c r="G9" s="62">
+      <c r="G9" s="55">
         <v>49478</v>
       </c>
-      <c r="H9" s="63"/>
-      <c r="I9" s="64"/>
-      <c r="J9" s="61"/>
-      <c r="K9" s="65"/>
-      <c r="L9" s="60"/>
-      <c r="M9" s="64"/>
-      <c r="N9" s="66"/>
-      <c r="O9" s="67"/>
-      <c r="P9" s="68"/>
-      <c r="Q9" s="69"/>
-      <c r="R9" s="70"/>
-      <c r="S9" s="70"/>
-      <c r="T9" s="70"/>
-      <c r="U9" s="71"/>
+      <c r="H9" s="56"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="58"/>
+      <c r="L9" s="53"/>
+      <c r="M9" s="57"/>
+      <c r="N9" s="59"/>
+      <c r="O9" s="60"/>
+      <c r="P9" s="61"/>
+      <c r="Q9" s="62"/>
+      <c r="R9" s="63"/>
+      <c r="S9" s="63"/>
+      <c r="T9" s="63"/>
+      <c r="U9" s="64"/>
     </row>
     <row r="10" spans="4:21" ht="24" x14ac:dyDescent="0.3">
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="29">
+      <c r="E10" s="25">
         <v>24</v>
       </c>
-      <c r="F10" s="30">
+      <c r="F10" s="26">
         <v>3992</v>
       </c>
-      <c r="G10" s="31">
+      <c r="G10" s="27">
         <v>3786</v>
       </c>
-      <c r="H10" s="40">
+      <c r="H10" s="36">
         <v>3.9499999999999999E-12</v>
       </c>
-      <c r="I10" s="41">
+      <c r="I10" s="37">
         <v>4.2399999999999997E-12</v>
       </c>
-      <c r="J10" s="33">
+      <c r="J10" s="29">
         <v>1.2100000000000001E-8</v>
       </c>
-      <c r="K10" s="34">
+      <c r="K10" s="30">
         <v>1.2100000000000001E-8</v>
       </c>
-      <c r="L10" s="35"/>
-      <c r="M10" s="41">
+      <c r="L10" s="31"/>
+      <c r="M10" s="37">
         <v>3.7299999999999997E-12</v>
       </c>
-      <c r="N10" s="41">
+      <c r="N10" s="37">
         <v>4.0399999999999997E-12</v>
       </c>
-      <c r="O10" s="33">
+      <c r="O10" s="29">
         <v>1.13E-8</v>
       </c>
-      <c r="P10" s="34">
+      <c r="P10" s="30">
         <v>1.13E-8</v>
       </c>
-      <c r="Q10" s="36"/>
-      <c r="R10" s="37">
+      <c r="Q10" s="32"/>
+      <c r="R10" s="33">
         <f>((H10-M10)/H10)</f>
         <v>5.5696202531645637E-2</v>
       </c>
-      <c r="S10" s="37">
+      <c r="S10" s="33">
         <f t="shared" ref="S10:U19" si="0">((I10-N10)/I10)</f>
         <v>4.7169811320754707E-2</v>
       </c>
-      <c r="T10" s="37">
+      <c r="T10" s="33">
         <f t="shared" si="0"/>
         <v>6.6115702479338886E-2</v>
       </c>
-      <c r="U10" s="38">
+      <c r="U10" s="34">
         <f t="shared" si="0"/>
         <v>6.6115702479338886E-2</v>
       </c>
     </row>
     <row r="11" spans="4:21" ht="24" x14ac:dyDescent="0.3">
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="10">
         <v>32</v>
       </c>
       <c r="F11" s="2">
@@ -1304,7 +1387,7 @@
       <c r="G11" s="5">
         <v>2333</v>
       </c>
-      <c r="H11" s="21">
+      <c r="H11" s="17">
         <v>6.5100000000000003E-12</v>
       </c>
       <c r="I11" s="6">
@@ -1313,7 +1396,7 @@
       <c r="J11" s="6">
         <v>1.77E-8</v>
       </c>
-      <c r="K11" s="16">
+      <c r="K11" s="12">
         <v>1.77E-8</v>
       </c>
       <c r="L11" s="3"/>
@@ -1326,88 +1409,88 @@
       <c r="O11" s="6">
         <v>1.4E-8</v>
       </c>
-      <c r="P11" s="16">
+      <c r="P11" s="12">
         <v>1.4E-8</v>
       </c>
       <c r="Q11" s="4"/>
-      <c r="R11" s="23">
+      <c r="R11" s="19">
         <f t="shared" ref="R11:R19" si="1">((H11-M11)/H11)</f>
         <v>0.17665130568356383</v>
       </c>
-      <c r="S11" s="23">
+      <c r="S11" s="19">
         <f t="shared" si="0"/>
         <v>0.33472803347280333</v>
       </c>
-      <c r="T11" s="23">
+      <c r="T11" s="19">
         <f t="shared" si="0"/>
         <v>0.20903954802259889</v>
       </c>
-      <c r="U11" s="24">
+      <c r="U11" s="20">
         <f t="shared" si="0"/>
         <v>0.20903954802259889</v>
       </c>
     </row>
     <row r="12" spans="4:21" ht="24" x14ac:dyDescent="0.3">
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="29">
+      <c r="E12" s="25">
         <v>8</v>
       </c>
-      <c r="F12" s="30">
+      <c r="F12" s="26">
         <v>311</v>
       </c>
-      <c r="G12" s="31">
+      <c r="G12" s="27">
         <v>270</v>
       </c>
-      <c r="H12" s="32">
+      <c r="H12" s="28">
         <v>2.9300000000000001E-13</v>
       </c>
-      <c r="I12" s="33">
+      <c r="I12" s="29">
         <v>2.5399999999999998E-13</v>
       </c>
-      <c r="J12" s="33">
+      <c r="J12" s="29">
         <v>7.78E-10</v>
       </c>
-      <c r="K12" s="34">
+      <c r="K12" s="30">
         <v>7.78E-10</v>
       </c>
-      <c r="L12" s="39"/>
-      <c r="M12" s="33">
+      <c r="L12" s="35"/>
+      <c r="M12" s="29">
         <v>2.7900000000000002E-13</v>
       </c>
-      <c r="N12" s="33">
+      <c r="N12" s="29">
         <v>2.2099999999999999E-13</v>
       </c>
-      <c r="O12" s="33">
+      <c r="O12" s="29">
         <v>7.8699999999999997E-10</v>
       </c>
-      <c r="P12" s="34">
+      <c r="P12" s="30">
         <v>7.8799999999999997E-10</v>
       </c>
-      <c r="Q12" s="36"/>
-      <c r="R12" s="37">
+      <c r="Q12" s="32"/>
+      <c r="R12" s="33">
         <f t="shared" si="1"/>
         <v>4.7781569965870276E-2</v>
       </c>
-      <c r="S12" s="37">
+      <c r="S12" s="33">
         <f t="shared" si="0"/>
         <v>0.12992125984251965</v>
       </c>
-      <c r="T12" s="37">
+      <c r="T12" s="33">
         <f t="shared" si="0"/>
         <v>-1.1568123393316155E-2</v>
       </c>
-      <c r="U12" s="38">
+      <c r="U12" s="34">
         <f t="shared" si="0"/>
         <v>-1.285347043701795E-2</v>
       </c>
     </row>
     <row r="13" spans="4:21" ht="24" x14ac:dyDescent="0.3">
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13" s="11">
         <v>8</v>
       </c>
       <c r="F13" s="2">
@@ -1416,7 +1499,7 @@
       <c r="G13" s="5">
         <v>290</v>
       </c>
-      <c r="H13" s="21">
+      <c r="H13" s="17">
         <v>3.8499999999999998E-13</v>
       </c>
       <c r="I13" s="6">
@@ -1425,7 +1508,7 @@
       <c r="J13" s="6">
         <v>1.15E-9</v>
       </c>
-      <c r="K13" s="16">
+      <c r="K13" s="12">
         <v>1.15E-9</v>
       </c>
       <c r="L13" s="3"/>
@@ -1438,88 +1521,88 @@
       <c r="O13" s="6">
         <v>1.15E-9</v>
       </c>
-      <c r="P13" s="16">
+      <c r="P13" s="12">
         <v>1.15E-9</v>
       </c>
       <c r="Q13" s="4"/>
-      <c r="R13" s="23">
+      <c r="R13" s="19">
         <f t="shared" si="1"/>
         <v>5.1948051948051731E-3</v>
       </c>
-      <c r="S13" s="23">
+      <c r="S13" s="19">
         <f t="shared" si="0"/>
         <v>5.1724137931034586E-2</v>
       </c>
-      <c r="T13" s="23">
+      <c r="T13" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U13" s="24">
+      <c r="U13" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="4:21" ht="24" x14ac:dyDescent="0.3">
-      <c r="D14" s="28" t="s">
+      <c r="D14" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="29">
+      <c r="E14" s="25">
         <v>107</v>
       </c>
-      <c r="F14" s="30">
+      <c r="F14" s="26">
         <v>1894</v>
       </c>
-      <c r="G14" s="31">
+      <c r="G14" s="27">
         <v>1174</v>
       </c>
-      <c r="H14" s="32">
+      <c r="H14" s="28">
         <v>1.9899999999999998E-12</v>
       </c>
-      <c r="I14" s="33">
+      <c r="I14" s="29">
         <v>1.9199999999999999E-12</v>
       </c>
-      <c r="J14" s="33">
+      <c r="J14" s="29">
         <v>5.2700000000000002E-9</v>
       </c>
-      <c r="K14" s="34">
+      <c r="K14" s="30">
         <v>5.2700000000000002E-9</v>
       </c>
-      <c r="L14" s="35"/>
-      <c r="M14" s="33">
+      <c r="L14" s="31"/>
+      <c r="M14" s="29">
         <v>1.6E-12</v>
       </c>
-      <c r="N14" s="33">
+      <c r="N14" s="29">
         <v>1.0599999999999999E-12</v>
       </c>
-      <c r="O14" s="33">
+      <c r="O14" s="29">
         <v>4.49E-9</v>
       </c>
-      <c r="P14" s="34">
+      <c r="P14" s="30">
         <v>4.49E-9</v>
       </c>
-      <c r="Q14" s="36"/>
-      <c r="R14" s="37">
+      <c r="Q14" s="32"/>
+      <c r="R14" s="33">
         <f t="shared" si="1"/>
         <v>0.19597989949748734</v>
       </c>
-      <c r="S14" s="37">
+      <c r="S14" s="33">
         <f t="shared" si="0"/>
         <v>0.44791666666666669</v>
       </c>
-      <c r="T14" s="37">
+      <c r="T14" s="33">
         <f t="shared" si="0"/>
         <v>0.14800759013282735</v>
       </c>
-      <c r="U14" s="38">
+      <c r="U14" s="34">
         <f t="shared" si="0"/>
         <v>0.14800759013282735</v>
       </c>
     </row>
     <row r="15" spans="4:21" ht="24" x14ac:dyDescent="0.3">
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15" s="11">
         <v>11</v>
       </c>
       <c r="F15" s="2">
@@ -1528,7 +1611,7 @@
       <c r="G15" s="5">
         <v>1805</v>
       </c>
-      <c r="H15" s="21">
+      <c r="H15" s="17">
         <v>3.8999999999999999E-12</v>
       </c>
       <c r="I15" s="6">
@@ -1537,7 +1620,7 @@
       <c r="J15" s="6">
         <v>1.15E-8</v>
       </c>
-      <c r="K15" s="16">
+      <c r="K15" s="12">
         <v>1.15E-8</v>
       </c>
       <c r="L15" s="3"/>
@@ -1550,88 +1633,88 @@
       <c r="O15" s="6">
         <v>5.6599999999999999E-9</v>
       </c>
-      <c r="P15" s="16">
+      <c r="P15" s="12">
         <v>5.6699999999999997E-9</v>
       </c>
       <c r="Q15" s="4"/>
-      <c r="R15" s="23">
+      <c r="R15" s="19">
         <f t="shared" si="1"/>
         <v>0.57179487179487176</v>
       </c>
-      <c r="S15" s="23">
+      <c r="S15" s="19">
         <f t="shared" si="0"/>
         <v>0.63543788187372707</v>
       </c>
-      <c r="T15" s="23">
+      <c r="T15" s="19">
         <f t="shared" si="0"/>
         <v>0.50782608695652176</v>
       </c>
-      <c r="U15" s="24">
+      <c r="U15" s="20">
         <f t="shared" si="0"/>
         <v>0.50695652173913053</v>
       </c>
     </row>
     <row r="16" spans="4:21" ht="24" x14ac:dyDescent="0.3">
-      <c r="D16" s="28" t="s">
+      <c r="D16" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="29">
+      <c r="E16" s="25">
         <v>392</v>
       </c>
-      <c r="F16" s="30">
+      <c r="F16" s="26">
         <v>11606</v>
       </c>
-      <c r="G16" s="31">
+      <c r="G16" s="27">
         <v>8594</v>
       </c>
-      <c r="H16" s="32">
+      <c r="H16" s="28">
         <v>1.8599999999999999E-11</v>
       </c>
-      <c r="I16" s="33">
+      <c r="I16" s="29">
         <v>8.8899999999999995E-12</v>
       </c>
-      <c r="J16" s="33">
+      <c r="J16" s="29">
         <v>3.6400000000000002E-8</v>
       </c>
-      <c r="K16" s="34">
+      <c r="K16" s="30">
         <v>3.6500000000000003E-8</v>
       </c>
-      <c r="L16" s="35"/>
-      <c r="M16" s="33">
+      <c r="L16" s="31"/>
+      <c r="M16" s="29">
         <v>1.56E-11</v>
       </c>
-      <c r="N16" s="33">
+      <c r="N16" s="29">
         <v>6.2500000000000002E-12</v>
       </c>
-      <c r="O16" s="33">
+      <c r="O16" s="29">
         <v>3.5999999999999998E-8</v>
       </c>
-      <c r="P16" s="34">
+      <c r="P16" s="30">
         <v>3.5999999999999998E-8</v>
       </c>
-      <c r="Q16" s="36"/>
-      <c r="R16" s="37">
+      <c r="Q16" s="32"/>
+      <c r="R16" s="33">
         <f t="shared" si="1"/>
         <v>0.16129032258064513</v>
       </c>
-      <c r="S16" s="37">
+      <c r="S16" s="33">
         <f t="shared" si="0"/>
         <v>0.29696287964004492</v>
       </c>
-      <c r="T16" s="37">
+      <c r="T16" s="33">
         <f t="shared" si="0"/>
         <v>1.0989010989011087E-2</v>
       </c>
-      <c r="U16" s="38">
+      <c r="U16" s="34">
         <f t="shared" si="0"/>
         <v>1.3698630136986424E-2</v>
       </c>
     </row>
-    <row r="17" spans="4:21" ht="24" x14ac:dyDescent="0.3">
-      <c r="D17" s="10" t="s">
+    <row r="17" spans="4:26" ht="24" x14ac:dyDescent="0.3">
+      <c r="D17" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="11">
         <v>256</v>
       </c>
       <c r="F17" s="2">
@@ -1640,7 +1723,7 @@
       <c r="G17" s="5">
         <v>5722</v>
       </c>
-      <c r="H17" s="21">
+      <c r="H17" s="17">
         <v>1.7799999999999999E-11</v>
       </c>
       <c r="I17" s="6">
@@ -1649,7 +1732,7 @@
       <c r="J17" s="6">
         <v>4.3800000000000002E-8</v>
       </c>
-      <c r="K17" s="16">
+      <c r="K17" s="12">
         <v>4.3800000000000002E-8</v>
       </c>
       <c r="L17" s="3"/>
@@ -1662,159 +1745,393 @@
       <c r="O17" s="6">
         <v>3.1200000000000001E-8</v>
       </c>
-      <c r="P17" s="16">
+      <c r="P17" s="12">
         <v>3.1200000000000001E-8</v>
       </c>
       <c r="Q17" s="4"/>
-      <c r="R17" s="23">
+      <c r="R17" s="19">
         <f t="shared" si="1"/>
         <v>0.36516853932584264</v>
       </c>
-      <c r="S17" s="23">
+      <c r="S17" s="19">
         <f t="shared" si="0"/>
         <v>0.69607843137254899</v>
       </c>
-      <c r="T17" s="23">
+      <c r="T17" s="19">
         <f t="shared" si="0"/>
         <v>0.28767123287671231</v>
       </c>
-      <c r="U17" s="24">
+      <c r="U17" s="20">
         <f t="shared" si="0"/>
         <v>0.28767123287671231</v>
       </c>
     </row>
-    <row r="18" spans="4:21" ht="24" x14ac:dyDescent="0.3">
-      <c r="D18" s="28" t="s">
+    <row r="18" spans="4:26" ht="22" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D18" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E18" s="29">
+      <c r="E18" s="25">
         <v>65</v>
       </c>
-      <c r="F18" s="30">
+      <c r="F18" s="26">
         <v>3807</v>
       </c>
-      <c r="G18" s="31">
+      <c r="G18" s="27">
         <v>1591</v>
       </c>
-      <c r="H18" s="32">
+      <c r="H18" s="28">
         <v>6.9200000000000004E-12</v>
       </c>
-      <c r="I18" s="33">
+      <c r="I18" s="29">
         <v>2.2100000000000001E-12</v>
       </c>
-      <c r="J18" s="33">
+      <c r="J18" s="29">
         <v>1.2499999999999999E-8</v>
       </c>
-      <c r="K18" s="34">
+      <c r="K18" s="30">
         <v>1.2499999999999999E-8</v>
       </c>
-      <c r="L18" s="35"/>
-      <c r="M18" s="33">
+      <c r="L18" s="31"/>
+      <c r="M18" s="29">
         <v>4.1100000000000001E-12</v>
       </c>
-      <c r="N18" s="33">
+      <c r="N18" s="29">
         <v>1.0700000000000001E-12</v>
       </c>
-      <c r="O18" s="33">
+      <c r="O18" s="29">
         <v>9.9599999999999995E-9</v>
       </c>
-      <c r="P18" s="34">
+      <c r="P18" s="30">
         <v>9.9599999999999995E-9</v>
       </c>
-      <c r="Q18" s="36"/>
-      <c r="R18" s="37">
+      <c r="Q18" s="32"/>
+      <c r="R18" s="33">
         <f t="shared" si="1"/>
         <v>0.40606936416184974</v>
       </c>
-      <c r="S18" s="37">
+      <c r="S18" s="33">
         <f t="shared" si="0"/>
         <v>0.51583710407239813</v>
       </c>
-      <c r="T18" s="37">
+      <c r="T18" s="33">
         <f t="shared" si="0"/>
         <v>0.20319999999999999</v>
       </c>
-      <c r="U18" s="38">
+      <c r="U18" s="34">
         <f t="shared" si="0"/>
         <v>0.20319999999999999</v>
       </c>
     </row>
-    <row r="19" spans="4:21" ht="25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D19" s="11" t="s">
+    <row r="19" spans="4:26" ht="25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D19" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="E19" s="15">
+      <c r="E19" s="74">
         <v>9</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="75">
         <v>905</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" s="76">
         <v>864</v>
       </c>
-      <c r="H19" s="22">
+      <c r="H19" s="18">
         <v>1.0599999999999999E-12</v>
       </c>
-      <c r="I19" s="12">
+      <c r="I19" s="9">
         <v>8.5100000000000001E-13</v>
       </c>
-      <c r="J19" s="12">
+      <c r="J19" s="9">
         <v>2.9199999999999998E-9</v>
       </c>
-      <c r="K19" s="17">
+      <c r="K19" s="13">
         <v>2.9199999999999998E-9</v>
       </c>
-      <c r="L19" s="20"/>
-      <c r="M19" s="12">
+      <c r="L19" s="16"/>
+      <c r="M19" s="9">
         <v>9.9200000000000001E-13</v>
       </c>
-      <c r="N19" s="18">
+      <c r="N19" s="14">
         <v>7.83E-13</v>
       </c>
-      <c r="O19" s="18">
+      <c r="O19" s="14">
         <v>2.5599999999999998E-9</v>
       </c>
-      <c r="P19" s="19">
+      <c r="P19" s="15">
         <v>2.5599999999999998E-9</v>
       </c>
-      <c r="Q19" s="27"/>
-      <c r="R19" s="25">
+      <c r="Q19" s="23"/>
+      <c r="R19" s="21">
         <f t="shared" si="1"/>
         <v>6.4150943396226331E-2</v>
       </c>
-      <c r="S19" s="25">
+      <c r="S19" s="21">
         <f t="shared" si="0"/>
         <v>7.9905992949471219E-2</v>
       </c>
-      <c r="T19" s="25">
+      <c r="T19" s="21">
         <f t="shared" si="0"/>
         <v>0.12328767123287672</v>
       </c>
-      <c r="U19" s="26">
+      <c r="U19" s="22">
         <f t="shared" si="0"/>
         <v>0.12328767123287672</v>
       </c>
     </row>
-    <row r="20" spans="4:21" ht="24" x14ac:dyDescent="0.3">
-      <c r="D20" s="1"/>
-      <c r="Q20" s="51" t="s">
+    <row r="20" spans="4:26" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="2">
+        <v>247</v>
+      </c>
+      <c r="F20" s="2">
+        <v>102653</v>
+      </c>
+      <c r="G20" s="2">
+        <v>98209</v>
+      </c>
+      <c r="H20" s="17">
+        <v>1.2500000000000001E-10</v>
+      </c>
+      <c r="I20" s="6">
+        <v>1.11E-10</v>
+      </c>
+      <c r="J20" s="6">
+        <v>2.8000000000000002E-7</v>
+      </c>
+      <c r="K20" s="12">
+        <v>2.8000000000000002E-7</v>
+      </c>
+      <c r="L20" s="3"/>
+      <c r="M20" s="6">
+        <v>1.02E-10</v>
+      </c>
+      <c r="N20" s="6">
+        <v>1.09E-10</v>
+      </c>
+      <c r="O20" s="6">
+        <v>2.7799999999999997E-7</v>
+      </c>
+      <c r="P20" s="12">
+        <v>2.7799999999999997E-7</v>
+      </c>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="21">
+        <f>((H20-M20)/H20)</f>
+        <v>0.18400000000000008</v>
+      </c>
+      <c r="S20" s="21">
+        <f t="shared" ref="S20:S23" si="2">((I20-N20)/I20)</f>
+        <v>1.801801801801807E-2</v>
+      </c>
+      <c r="T20" s="21">
+        <f t="shared" ref="T20:T23" si="3">((J20-O20)/J20)</f>
+        <v>7.1428571428573005E-3</v>
+      </c>
+      <c r="U20" s="22">
+        <f t="shared" ref="U20:U23" si="4">((K20-P20)/K20)</f>
+        <v>7.1428571428573005E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="4:26" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="17">
+        <v>3.0099999999999998E-11</v>
+      </c>
+      <c r="I21" s="6">
+        <v>2.6499999999999999E-11</v>
+      </c>
+      <c r="J21" s="6">
+        <v>7.4600000000000006E-8</v>
+      </c>
+      <c r="K21" s="12">
+        <v>7.4600000000000006E-8</v>
+      </c>
+      <c r="L21" s="72"/>
+      <c r="M21" s="17">
+        <v>3.1000000000000003E-11</v>
+      </c>
+      <c r="N21" s="6">
+        <v>2.5699999999999999E-11</v>
+      </c>
+      <c r="O21" s="6">
+        <v>6.9100000000000003E-8</v>
+      </c>
+      <c r="P21" s="12">
+        <v>6.9199999999999998E-8</v>
+      </c>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="21">
+        <f>((H21-M21)/H21)</f>
+        <v>-2.9900332225913779E-2</v>
+      </c>
+      <c r="S21" s="21">
+        <f t="shared" ref="S21" si="5">((I21-N21)/I21)</f>
+        <v>3.0188679245283012E-2</v>
+      </c>
+      <c r="T21" s="21">
+        <f t="shared" ref="T21" si="6">((J21-O21)/J21)</f>
+        <v>7.3726541554959821E-2</v>
+      </c>
+      <c r="U21" s="22">
+        <f t="shared" ref="U21" si="7">((K21-P21)/K21)</f>
+        <v>7.2386058981233348E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="4:26" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D22" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="17">
+        <v>1.7300000000000001E-11</v>
+      </c>
+      <c r="I22" s="6">
+        <v>1.27E-11</v>
+      </c>
+      <c r="J22" s="6">
+        <v>4.3499999999999999E-8</v>
+      </c>
+      <c r="K22" s="12">
+        <v>4.36E-8</v>
+      </c>
+      <c r="M22" s="77">
+        <v>1.58E-11</v>
+      </c>
+      <c r="N22" s="6">
+        <v>1.1600000000000001E-11</v>
+      </c>
+      <c r="O22" s="6">
+        <v>4.1899999999999998E-8</v>
+      </c>
+      <c r="P22" s="12">
+        <v>4.1899999999999998E-8</v>
+      </c>
+      <c r="Q22" s="4"/>
+      <c r="R22" s="21">
+        <f t="shared" ref="R22" si="8">((H22-M22)/H22)</f>
+        <v>8.6705202312138796E-2</v>
+      </c>
+      <c r="S22" s="21">
+        <f t="shared" ref="S22" si="9">((I22-N22)/I22)</f>
+        <v>8.6614173228346428E-2</v>
+      </c>
+      <c r="T22" s="21">
+        <f t="shared" ref="T22" si="10">((J22-O22)/J22)</f>
+        <v>3.6781609195402326E-2</v>
+      </c>
+      <c r="U22" s="22">
+        <f t="shared" ref="U22" si="11">((K22-P22)/K22)</f>
+        <v>3.8990825688073438E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="4:26" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D23" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="2">
+        <v>2048</v>
+      </c>
+      <c r="F23" s="2">
+        <v>41788</v>
+      </c>
+      <c r="G23" s="2">
+        <v>44958</v>
+      </c>
+      <c r="H23" s="17">
+        <v>4.6999999999999999E-11</v>
+      </c>
+      <c r="I23" s="6">
+        <v>5.0400000000000002E-11</v>
+      </c>
+      <c r="J23" s="6">
+        <v>1.23E-7</v>
+      </c>
+      <c r="K23" s="12">
+        <v>1.23E-7</v>
+      </c>
+      <c r="L23" s="3"/>
+      <c r="M23" s="6">
+        <v>9.7600000000000004E-11</v>
+      </c>
+      <c r="N23" s="6">
+        <v>5.01E-11</v>
+      </c>
+      <c r="O23" s="6">
+        <v>1.3300000000000001E-7</v>
+      </c>
+      <c r="P23" s="12">
+        <v>1.3300000000000001E-7</v>
+      </c>
+      <c r="Q23" s="4"/>
+      <c r="R23" s="21">
+        <f t="shared" ref="R20:R23" si="12">((H23-M23)/H23)</f>
+        <v>-1.0765957446808512</v>
+      </c>
+      <c r="S23" s="21">
+        <f t="shared" si="2"/>
+        <v>5.9523809523809833E-3</v>
+      </c>
+      <c r="T23" s="21">
+        <f t="shared" si="3"/>
+        <v>-8.1300813008130163E-2</v>
+      </c>
+      <c r="U23" s="22">
+        <f t="shared" si="4"/>
+        <v>-8.1300813008130163E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="4:26" ht="24" x14ac:dyDescent="0.3">
+      <c r="D24" s="1"/>
+      <c r="E24" s="71"/>
+      <c r="F24" s="71"/>
+      <c r="G24" s="71"/>
+      <c r="H24" s="71"/>
+      <c r="Q24" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="R20" s="52">
-        <f>AVERAGE(R10:R19)</f>
-        <v>0.20497778241328074</v>
-      </c>
-      <c r="S20" s="52">
-        <f>AVERAGE(S10:S19)</f>
-        <v>0.32356821991419693</v>
-      </c>
-      <c r="T20" s="52">
-        <f>AVERAGE(T10:T19)</f>
-        <v>0.1544568719296571</v>
-      </c>
-      <c r="U20" s="52">
-        <f>AVERAGE(U10:U19)</f>
-        <v>0.15451234261834532</v>
+      <c r="R24" s="48">
+        <f>AVERAGE(R10:R23)</f>
+        <v>8.6713353538441534E-2</v>
+      </c>
+      <c r="S24" s="48">
+        <f t="shared" ref="S24:T24" si="13">AVERAGE(S10:S23)</f>
+        <v>0.24117538932757127</v>
+      </c>
+      <c r="T24" s="48">
+        <f t="shared" si="13"/>
+        <v>0.1129227795844043</v>
+      </c>
+      <c r="U24" s="48">
+        <f>AVERAGE(U10:U23)</f>
+        <v>0.11302445392767767</v>
+      </c>
+    </row>
+    <row r="26" spans="4:26" x14ac:dyDescent="0.2">
+      <c r="Z26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="4:26" x14ac:dyDescent="0.2">
+      <c r="F30" s="68"/>
+    </row>
+    <row r="42" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D42" s="69"/>
+    </row>
+    <row r="43" spans="4:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="D43" s="70"/>
+    </row>
+    <row r="52" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I52" s="68" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1823,6 +2140,9 @@
     <mergeCell ref="M7:P7"/>
     <mergeCell ref="R7:U7"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="I52" r:id="rId1" xr:uid="{73DB033F-362A-944F-B285-69242C4267BF}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
shifting to .ys/ aoi cells analysis
</commit_message>
<xml_diff>
--- a/dynamic_power_analysis/code/OpenSTA_report_power/dynamic_power_analysis.xlsx
+++ b/dynamic_power_analysis/code/OpenSTA_report_power/dynamic_power_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/youssef/Desktop/EDA/Dynamic_Power_Clock_Gating/dynamic_power_analysis/code/OpenSTA_report_power/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74E8709-1F65-4343-B09D-5004A256FCA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F299432-3310-554C-B0B3-D3280E0A6891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="25600" windowHeight="14160" xr2:uid="{42F2CD03-9D47-9445-8059-7D7C13E91239}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{42F2CD03-9D47-9445-8059-7D7C13E91239}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="53">
   <si>
     <t xml:space="preserve">module </t>
   </si>
@@ -138,13 +138,67 @@
   </si>
   <si>
     <t>riscv_top_151</t>
+  </si>
+  <si>
+    <t>module</t>
+  </si>
+  <si>
+    <t>clock gates</t>
+  </si>
+  <si>
+    <t>cells before</t>
+  </si>
+  <si>
+    <t>cells difference</t>
+  </si>
+  <si>
+    <t>cells after</t>
+  </si>
+  <si>
+    <t>a211oi_1 before</t>
+  </si>
+  <si>
+    <t>a21oi_1 before</t>
+  </si>
+  <si>
+    <t>a22o_1 before</t>
+  </si>
+  <si>
+    <t>a22oi_1 before</t>
+  </si>
+  <si>
+    <t>a211oi_1 after</t>
+  </si>
+  <si>
+    <t>a21oi_1 after</t>
+  </si>
+  <si>
+    <t>a22o_1 after</t>
+  </si>
+  <si>
+    <t>a22oi_1 after</t>
+  </si>
+  <si>
+    <t>aoi/ao difference</t>
+  </si>
+  <si>
+    <t>aes256</t>
+  </si>
+  <si>
+    <t>PPU</t>
+  </si>
+  <si>
+    <t>des</t>
+  </si>
+  <si>
+    <t>sbox</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -188,25 +242,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <i/>
       <sz val="20"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -221,16 +259,45 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color rgb="FF24292E"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="20"/>
       <color theme="1"/>
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="16"/>
+      <sz val="20"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
       <color theme="1"/>
-      <name val="Helvetica"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -271,7 +338,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -584,49 +651,76 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="6" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="6" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -634,23 +728,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="11" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -662,20 +744,82 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="8" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="8" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="8" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="8" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="8" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="8" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="9" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="12" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="12" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -992,35 +1136,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3E8C89-AABD-1C41-B99B-18B443C74BC8}">
-  <dimension ref="C6:Z42"/>
+  <dimension ref="C6:Z77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G11" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="43" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="23.1640625" customWidth="1"/>
-    <col min="5" max="5" width="30.33203125" customWidth="1"/>
+    <col min="4" max="4" width="44.1640625" style="46" customWidth="1"/>
+    <col min="5" max="5" width="33.5" customWidth="1"/>
     <col min="6" max="6" width="20.6640625" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.33203125" customWidth="1"/>
-    <col min="9" max="9" width="20" customWidth="1"/>
-    <col min="10" max="10" width="21.5" customWidth="1"/>
-    <col min="11" max="12" width="21" customWidth="1"/>
-    <col min="13" max="13" width="20.33203125" customWidth="1"/>
-    <col min="14" max="14" width="19" customWidth="1"/>
-    <col min="15" max="15" width="17.1640625" customWidth="1"/>
-    <col min="16" max="16" width="10.6640625" customWidth="1"/>
-    <col min="17" max="17" width="24.33203125" customWidth="1"/>
+    <col min="7" max="7" width="25.33203125" customWidth="1"/>
+    <col min="8" max="8" width="26.33203125" customWidth="1"/>
+    <col min="9" max="9" width="25.83203125" customWidth="1"/>
+    <col min="10" max="10" width="25.33203125" customWidth="1"/>
+    <col min="11" max="11" width="24.83203125" customWidth="1"/>
+    <col min="12" max="12" width="26" customWidth="1"/>
+    <col min="13" max="13" width="26.1640625" customWidth="1"/>
+    <col min="14" max="14" width="23.6640625" customWidth="1"/>
+    <col min="15" max="15" width="24.1640625" customWidth="1"/>
+    <col min="16" max="16" width="24.6640625" customWidth="1"/>
+    <col min="17" max="17" width="28.1640625" customWidth="1"/>
     <col min="18" max="18" width="15" customWidth="1"/>
     <col min="19" max="19" width="13.5" customWidth="1"/>
     <col min="20" max="20" width="12" customWidth="1"/>
     <col min="21" max="21" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="3:21" ht="25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D6" s="1"/>
+    <row r="6" spans="3:21" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -1034,210 +1178,206 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="3:21" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="60" t="s">
+    <row r="7" spans="3:21" s="46" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H7" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="61"/>
-      <c r="J7" s="61"/>
-      <c r="K7" s="61"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="61" t="s">
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="N7" s="61"/>
-      <c r="O7" s="61"/>
-      <c r="P7" s="62"/>
-      <c r="Q7" s="12"/>
-      <c r="R7" s="61" t="s">
+      <c r="N7" s="32"/>
+      <c r="O7" s="32"/>
+      <c r="P7" s="33"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="S7" s="61"/>
-      <c r="T7" s="61"/>
-      <c r="U7" s="62"/>
-    </row>
-    <row r="8" spans="3:21" ht="25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D8" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" s="21" t="s">
+      <c r="S7" s="32"/>
+      <c r="T7" s="32"/>
+      <c r="U7" s="33"/>
+    </row>
+    <row r="8" spans="3:21" s="46" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D8" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="24" t="s">
+      <c r="H8" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="25" t="s">
+      <c r="I8" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="J8" s="22" t="s">
+      <c r="J8" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="26" t="s">
+      <c r="K8" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="L8" s="27"/>
-      <c r="M8" s="25" t="s">
+      <c r="L8" s="68"/>
+      <c r="M8" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="N8" s="25" t="s">
+      <c r="N8" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="O8" s="26" t="s">
+      <c r="O8" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="P8" s="28" t="s">
+      <c r="P8" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="Q8" s="29"/>
-      <c r="R8" s="25" t="s">
+      <c r="Q8" s="70"/>
+      <c r="R8" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="S8" s="24" t="s">
+      <c r="S8" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="T8" s="26" t="s">
+      <c r="T8" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="U8" s="28" t="s">
+      <c r="U8" s="69" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="3:21" ht="24" x14ac:dyDescent="0.3">
-      <c r="C9" s="52">
+    <row r="9" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C9" s="25">
         <v>1</v>
       </c>
-      <c r="D9" s="39" t="s">
+      <c r="D9" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="40">
+      <c r="E9" s="19">
         <v>513</v>
       </c>
-      <c r="F9" s="40">
+      <c r="F9" s="19">
         <v>55531</v>
       </c>
-      <c r="G9" s="40">
+      <c r="G9" s="19">
         <v>49478</v>
       </c>
-      <c r="H9" s="41">
+      <c r="H9" s="20">
         <v>4.0899999999999998E-10</v>
       </c>
-      <c r="I9" s="41">
+      <c r="I9" s="20">
         <v>7.5300000000000001E-11</v>
       </c>
-      <c r="J9" s="42">
+      <c r="J9" s="21">
         <v>1.5800000000000001E-7</v>
       </c>
-      <c r="K9" s="42">
+      <c r="K9" s="21">
         <v>1.5800000000000001E-7</v>
       </c>
-      <c r="L9" s="40"/>
-      <c r="M9" s="41">
+      <c r="L9" s="19"/>
+      <c r="M9" s="20">
         <v>1.8899999999999999E-10</v>
       </c>
-      <c r="N9" s="41">
+      <c r="N9" s="20">
         <v>5.3399999999999998E-11</v>
       </c>
-      <c r="O9" s="42">
+      <c r="O9" s="21">
         <v>1.5599999999999999E-7</v>
       </c>
-      <c r="P9" s="42">
+      <c r="P9" s="21">
         <v>1.5699999999999999E-7</v>
       </c>
-      <c r="Q9" s="43"/>
-      <c r="R9" s="44">
+      <c r="Q9" s="22"/>
+      <c r="R9" s="34">
         <f>((H9-M9)/H9)</f>
         <v>0.53789731051344747</v>
       </c>
-      <c r="S9" s="44">
+      <c r="S9" s="34">
         <f t="shared" ref="S9" si="0">((I9-N9)/I9)</f>
         <v>0.2908366533864542</v>
       </c>
-      <c r="T9" s="44">
+      <c r="T9" s="34">
         <f t="shared" ref="T9" si="1">((J9-O9)/J9)</f>
         <v>1.2658227848101378E-2</v>
       </c>
-      <c r="U9" s="45">
+      <c r="U9" s="35">
         <f t="shared" ref="U9" si="2">((K9-P9)/K9)</f>
         <v>6.3291139240507725E-3</v>
       </c>
     </row>
-    <row r="10" spans="3:21" ht="24" x14ac:dyDescent="0.3">
-      <c r="C10" s="53">
+    <row r="10" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C10" s="26">
         <v>2</v>
       </c>
-      <c r="D10" s="46" t="s">
+      <c r="D10" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="31">
+      <c r="E10" s="12">
         <v>24</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="4">
         <v>3992</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="4">
         <v>3786</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H10" s="6">
         <v>3.9499999999999999E-12</v>
       </c>
-      <c r="I10" s="10">
+      <c r="I10" s="6">
         <v>4.2399999999999997E-12</v>
       </c>
-      <c r="J10" s="7">
+      <c r="J10" s="5">
         <v>1.2100000000000001E-8</v>
       </c>
-      <c r="K10" s="7">
+      <c r="K10" s="5">
         <v>1.2100000000000001E-8</v>
       </c>
-      <c r="L10" s="6"/>
-      <c r="M10" s="10">
+      <c r="L10" s="4"/>
+      <c r="M10" s="6">
         <v>3.7299999999999997E-12</v>
       </c>
-      <c r="N10" s="10">
+      <c r="N10" s="6">
         <v>4.0399999999999997E-12</v>
       </c>
-      <c r="O10" s="7">
+      <c r="O10" s="5">
         <v>1.13E-8</v>
       </c>
-      <c r="P10" s="7">
+      <c r="P10" s="5">
         <v>1.13E-8</v>
       </c>
-      <c r="Q10" s="32"/>
-      <c r="R10" s="8">
+      <c r="Q10" s="13"/>
+      <c r="R10" s="36">
         <f>((H10-M10)/H10)</f>
         <v>5.5696202531645637E-2</v>
       </c>
-      <c r="S10" s="8">
+      <c r="S10" s="36">
         <f t="shared" ref="S10:U19" si="3">((I10-N10)/I10)</f>
         <v>4.7169811320754707E-2</v>
       </c>
-      <c r="T10" s="8">
+      <c r="T10" s="36">
         <f t="shared" si="3"/>
         <v>6.6115702479338886E-2</v>
       </c>
-      <c r="U10" s="9">
+      <c r="U10" s="37">
         <f t="shared" si="3"/>
         <v>6.6115702479338886E-2</v>
       </c>
     </row>
-    <row r="11" spans="3:21" ht="24" x14ac:dyDescent="0.3">
-      <c r="C11" s="53">
+    <row r="11" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C11" s="26">
         <v>3</v>
       </c>
-      <c r="D11" s="47" t="s">
+      <c r="D11" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="30">
+      <c r="E11" s="11">
         <v>32</v>
       </c>
       <c r="F11" s="2">
@@ -1271,91 +1411,91 @@
       <c r="P11" s="3">
         <v>1.4E-8</v>
       </c>
-      <c r="Q11" s="33"/>
-      <c r="R11" s="4">
+      <c r="Q11" s="14"/>
+      <c r="R11" s="38">
         <f t="shared" ref="R11:R19" si="4">((H11-M11)/H11)</f>
         <v>0.17665130568356383</v>
       </c>
-      <c r="S11" s="4">
+      <c r="S11" s="38">
         <f t="shared" si="3"/>
         <v>0.33472803347280333</v>
       </c>
-      <c r="T11" s="4">
+      <c r="T11" s="38">
         <f t="shared" si="3"/>
         <v>0.20903954802259889</v>
       </c>
-      <c r="U11" s="5">
+      <c r="U11" s="39">
         <f t="shared" si="3"/>
         <v>0.20903954802259889</v>
       </c>
     </row>
-    <row r="12" spans="3:21" ht="24" x14ac:dyDescent="0.3">
-      <c r="C12" s="53">
+    <row r="12" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C12" s="26">
         <v>4</v>
       </c>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="31">
+      <c r="E12" s="12">
         <v>8</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="4">
         <v>311</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="4">
         <v>270</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="5">
         <v>2.9300000000000001E-13</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I12" s="5">
         <v>2.5399999999999998E-13</v>
       </c>
-      <c r="J12" s="7">
+      <c r="J12" s="5">
         <v>7.78E-10</v>
       </c>
-      <c r="K12" s="7">
+      <c r="K12" s="5">
         <v>7.78E-10</v>
       </c>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7">
+      <c r="L12" s="5"/>
+      <c r="M12" s="5">
         <v>2.7900000000000002E-13</v>
       </c>
-      <c r="N12" s="7">
+      <c r="N12" s="5">
         <v>2.2099999999999999E-13</v>
       </c>
-      <c r="O12" s="7">
+      <c r="O12" s="5">
         <v>7.8699999999999997E-10</v>
       </c>
-      <c r="P12" s="7">
+      <c r="P12" s="5">
         <v>7.8799999999999997E-10</v>
       </c>
-      <c r="Q12" s="32"/>
-      <c r="R12" s="8">
+      <c r="Q12" s="13"/>
+      <c r="R12" s="36">
         <f t="shared" si="4"/>
         <v>4.7781569965870276E-2</v>
       </c>
-      <c r="S12" s="8">
+      <c r="S12" s="36">
         <f t="shared" si="3"/>
         <v>0.12992125984251965</v>
       </c>
-      <c r="T12" s="8">
+      <c r="T12" s="36">
         <f t="shared" si="3"/>
         <v>-1.1568123393316155E-2</v>
       </c>
-      <c r="U12" s="9">
+      <c r="U12" s="37">
         <f t="shared" si="3"/>
         <v>-1.285347043701795E-2</v>
       </c>
     </row>
-    <row r="13" spans="3:21" ht="24" x14ac:dyDescent="0.3">
-      <c r="C13" s="53">
+    <row r="13" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C13" s="26">
         <v>5</v>
       </c>
-      <c r="D13" s="48" t="s">
+      <c r="D13" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="34">
+      <c r="E13" s="15">
         <v>8</v>
       </c>
       <c r="F13" s="2">
@@ -1389,91 +1529,91 @@
       <c r="P13" s="3">
         <v>1.15E-9</v>
       </c>
-      <c r="Q13" s="33"/>
-      <c r="R13" s="4">
+      <c r="Q13" s="14"/>
+      <c r="R13" s="38">
         <f t="shared" si="4"/>
         <v>5.1948051948051731E-3</v>
       </c>
-      <c r="S13" s="4">
+      <c r="S13" s="38">
         <f t="shared" si="3"/>
         <v>5.1724137931034586E-2</v>
       </c>
-      <c r="T13" s="4">
+      <c r="T13" s="38">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="U13" s="5">
+      <c r="U13" s="39">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="3:21" ht="24" x14ac:dyDescent="0.3">
-      <c r="C14" s="53">
+    <row r="14" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C14" s="26">
         <v>6</v>
       </c>
-      <c r="D14" s="46" t="s">
+      <c r="D14" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="31">
+      <c r="E14" s="12">
         <v>107</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="4">
         <v>1894</v>
       </c>
-      <c r="G14" s="6">
+      <c r="G14" s="4">
         <v>1174</v>
       </c>
-      <c r="H14" s="7">
+      <c r="H14" s="5">
         <v>1.9899999999999998E-12</v>
       </c>
-      <c r="I14" s="7">
+      <c r="I14" s="5">
         <v>1.9199999999999999E-12</v>
       </c>
-      <c r="J14" s="7">
+      <c r="J14" s="5">
         <v>5.2700000000000002E-9</v>
       </c>
-      <c r="K14" s="7">
+      <c r="K14" s="5">
         <v>5.2700000000000002E-9</v>
       </c>
-      <c r="L14" s="6"/>
-      <c r="M14" s="7">
+      <c r="L14" s="4"/>
+      <c r="M14" s="5">
         <v>1.6E-12</v>
       </c>
-      <c r="N14" s="7">
+      <c r="N14" s="5">
         <v>1.0599999999999999E-12</v>
       </c>
-      <c r="O14" s="7">
+      <c r="O14" s="5">
         <v>4.49E-9</v>
       </c>
-      <c r="P14" s="7">
+      <c r="P14" s="5">
         <v>4.49E-9</v>
       </c>
-      <c r="Q14" s="32"/>
-      <c r="R14" s="8">
+      <c r="Q14" s="13"/>
+      <c r="R14" s="36">
         <f t="shared" si="4"/>
         <v>0.19597989949748734</v>
       </c>
-      <c r="S14" s="8">
+      <c r="S14" s="36">
         <f t="shared" si="3"/>
         <v>0.44791666666666669</v>
       </c>
-      <c r="T14" s="8">
+      <c r="T14" s="36">
         <f t="shared" si="3"/>
         <v>0.14800759013282735</v>
       </c>
-      <c r="U14" s="9">
+      <c r="U14" s="37">
         <f t="shared" si="3"/>
         <v>0.14800759013282735</v>
       </c>
     </row>
-    <row r="15" spans="3:21" ht="24" x14ac:dyDescent="0.3">
-      <c r="C15" s="53">
+    <row r="15" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C15" s="26">
         <v>7</v>
       </c>
-      <c r="D15" s="48" t="s">
+      <c r="D15" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="34">
+      <c r="E15" s="15">
         <v>11</v>
       </c>
       <c r="F15" s="2">
@@ -1507,91 +1647,91 @@
       <c r="P15" s="3">
         <v>5.6699999999999997E-9</v>
       </c>
-      <c r="Q15" s="33"/>
-      <c r="R15" s="4">
+      <c r="Q15" s="14"/>
+      <c r="R15" s="38">
         <f t="shared" si="4"/>
         <v>0.57179487179487176</v>
       </c>
-      <c r="S15" s="4">
+      <c r="S15" s="38">
         <f t="shared" si="3"/>
         <v>0.63543788187372707</v>
       </c>
-      <c r="T15" s="4">
+      <c r="T15" s="38">
         <f t="shared" si="3"/>
         <v>0.50782608695652176</v>
       </c>
-      <c r="U15" s="5">
+      <c r="U15" s="39">
         <f t="shared" si="3"/>
         <v>0.50695652173913053</v>
       </c>
     </row>
-    <row r="16" spans="3:21" ht="24" x14ac:dyDescent="0.3">
-      <c r="C16" s="53">
+    <row r="16" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C16" s="26">
         <v>8</v>
       </c>
-      <c r="D16" s="46" t="s">
+      <c r="D16" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="31">
+      <c r="E16" s="12">
         <v>392</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="4">
         <v>11606</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="4">
         <v>8594</v>
       </c>
-      <c r="H16" s="7">
+      <c r="H16" s="5">
         <v>1.8599999999999999E-11</v>
       </c>
-      <c r="I16" s="7">
+      <c r="I16" s="5">
         <v>8.8899999999999995E-12</v>
       </c>
-      <c r="J16" s="7">
+      <c r="J16" s="5">
         <v>3.6400000000000002E-8</v>
       </c>
-      <c r="K16" s="7">
+      <c r="K16" s="5">
         <v>3.6500000000000003E-8</v>
       </c>
-      <c r="L16" s="6"/>
-      <c r="M16" s="7">
+      <c r="L16" s="4"/>
+      <c r="M16" s="5">
         <v>1.56E-11</v>
       </c>
-      <c r="N16" s="7">
+      <c r="N16" s="5">
         <v>6.2500000000000002E-12</v>
       </c>
-      <c r="O16" s="7">
+      <c r="O16" s="5">
         <v>3.5999999999999998E-8</v>
       </c>
-      <c r="P16" s="7">
+      <c r="P16" s="5">
         <v>3.5999999999999998E-8</v>
       </c>
-      <c r="Q16" s="32"/>
-      <c r="R16" s="8">
+      <c r="Q16" s="13"/>
+      <c r="R16" s="36">
         <f t="shared" si="4"/>
         <v>0.16129032258064513</v>
       </c>
-      <c r="S16" s="8">
+      <c r="S16" s="36">
         <f t="shared" si="3"/>
         <v>0.29696287964004492</v>
       </c>
-      <c r="T16" s="8">
+      <c r="T16" s="36">
         <f t="shared" si="3"/>
         <v>1.0989010989011087E-2</v>
       </c>
-      <c r="U16" s="9">
+      <c r="U16" s="37">
         <f t="shared" si="3"/>
         <v>1.3698630136986424E-2</v>
       </c>
     </row>
-    <row r="17" spans="3:26" ht="24" x14ac:dyDescent="0.3">
-      <c r="C17" s="53">
+    <row r="17" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="C17" s="26">
         <v>9</v>
       </c>
-      <c r="D17" s="48" t="s">
+      <c r="D17" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="34">
+      <c r="E17" s="15">
         <v>256</v>
       </c>
       <c r="F17" s="2">
@@ -1625,91 +1765,91 @@
       <c r="P17" s="3">
         <v>3.1200000000000001E-8</v>
       </c>
-      <c r="Q17" s="33"/>
-      <c r="R17" s="4">
+      <c r="Q17" s="14"/>
+      <c r="R17" s="38">
         <f t="shared" si="4"/>
         <v>0.36516853932584264</v>
       </c>
-      <c r="S17" s="4">
+      <c r="S17" s="38">
         <f t="shared" si="3"/>
         <v>0.69607843137254899</v>
       </c>
-      <c r="T17" s="4">
+      <c r="T17" s="38">
         <f t="shared" si="3"/>
         <v>0.28767123287671231</v>
       </c>
-      <c r="U17" s="5">
+      <c r="U17" s="39">
         <f t="shared" si="3"/>
         <v>0.28767123287671231</v>
       </c>
     </row>
     <row r="18" spans="3:26" ht="22" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="53">
+      <c r="C18" s="26">
         <v>10</v>
       </c>
-      <c r="D18" s="46" t="s">
+      <c r="D18" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="E18" s="31">
+      <c r="E18" s="12">
         <v>65</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="4">
         <v>3807</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G18" s="4">
         <v>1591</v>
       </c>
-      <c r="H18" s="7">
+      <c r="H18" s="5">
         <v>6.9200000000000004E-12</v>
       </c>
-      <c r="I18" s="7">
+      <c r="I18" s="5">
         <v>2.2100000000000001E-12</v>
       </c>
-      <c r="J18" s="7">
+      <c r="J18" s="5">
         <v>1.2499999999999999E-8</v>
       </c>
-      <c r="K18" s="7">
+      <c r="K18" s="5">
         <v>1.2499999999999999E-8</v>
       </c>
-      <c r="L18" s="6"/>
-      <c r="M18" s="7">
+      <c r="L18" s="4"/>
+      <c r="M18" s="5">
         <v>4.1100000000000001E-12</v>
       </c>
-      <c r="N18" s="7">
+      <c r="N18" s="5">
         <v>1.0700000000000001E-12</v>
       </c>
-      <c r="O18" s="7">
+      <c r="O18" s="5">
         <v>9.9599999999999995E-9</v>
       </c>
-      <c r="P18" s="7">
+      <c r="P18" s="5">
         <v>9.9599999999999995E-9</v>
       </c>
-      <c r="Q18" s="32"/>
-      <c r="R18" s="8">
+      <c r="Q18" s="13"/>
+      <c r="R18" s="36">
         <f t="shared" si="4"/>
         <v>0.40606936416184974</v>
       </c>
-      <c r="S18" s="8">
+      <c r="S18" s="36">
         <f t="shared" si="3"/>
         <v>0.51583710407239813</v>
       </c>
-      <c r="T18" s="8">
+      <c r="T18" s="36">
         <f t="shared" si="3"/>
         <v>0.20319999999999999</v>
       </c>
-      <c r="U18" s="9">
+      <c r="U18" s="37">
         <f t="shared" si="3"/>
         <v>0.20319999999999999</v>
       </c>
     </row>
-    <row r="19" spans="3:26" ht="24" x14ac:dyDescent="0.3">
-      <c r="C19" s="53">
+    <row r="19" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="C19" s="26">
         <v>11</v>
       </c>
-      <c r="D19" s="48" t="s">
+      <c r="D19" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="E19" s="34">
+      <c r="E19" s="15">
         <v>9</v>
       </c>
       <c r="F19" s="2">
@@ -1743,88 +1883,88 @@
       <c r="P19" s="3">
         <v>2.5599999999999998E-9</v>
       </c>
-      <c r="Q19" s="33"/>
-      <c r="R19" s="4">
+      <c r="Q19" s="14"/>
+      <c r="R19" s="38">
         <f t="shared" si="4"/>
         <v>6.4150943396226331E-2</v>
       </c>
-      <c r="S19" s="4">
+      <c r="S19" s="38">
         <f t="shared" si="3"/>
         <v>7.9905992949471219E-2</v>
       </c>
-      <c r="T19" s="4">
+      <c r="T19" s="38">
         <f t="shared" si="3"/>
         <v>0.12328767123287672</v>
       </c>
-      <c r="U19" s="5">
+      <c r="U19" s="39">
         <f t="shared" si="3"/>
         <v>0.12328767123287672</v>
       </c>
     </row>
-    <row r="20" spans="3:26" ht="24" x14ac:dyDescent="0.3">
-      <c r="C20" s="53">
+    <row r="20" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="C20" s="26">
         <v>12</v>
       </c>
-      <c r="D20" s="55" t="s">
+      <c r="D20" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="4">
         <v>247</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="4">
         <v>102653</v>
       </c>
-      <c r="G20" s="6">
+      <c r="G20" s="4">
         <v>98209</v>
       </c>
-      <c r="H20" s="7">
+      <c r="H20" s="5">
         <v>1.2500000000000001E-10</v>
       </c>
-      <c r="I20" s="7">
+      <c r="I20" s="5">
         <v>1.11E-10</v>
       </c>
-      <c r="J20" s="7">
+      <c r="J20" s="5">
         <v>2.8000000000000002E-7</v>
       </c>
-      <c r="K20" s="7">
+      <c r="K20" s="5">
         <v>2.8000000000000002E-7</v>
       </c>
-      <c r="L20" s="6"/>
-      <c r="M20" s="7">
+      <c r="L20" s="4"/>
+      <c r="M20" s="5">
         <v>1.02E-10</v>
       </c>
-      <c r="N20" s="7">
+      <c r="N20" s="5">
         <v>1.09E-10</v>
       </c>
-      <c r="O20" s="7">
+      <c r="O20" s="5">
         <v>2.7799999999999997E-7</v>
       </c>
-      <c r="P20" s="7">
+      <c r="P20" s="5">
         <v>2.7799999999999997E-7</v>
       </c>
-      <c r="Q20" s="32"/>
-      <c r="R20" s="8">
+      <c r="Q20" s="13"/>
+      <c r="R20" s="36">
         <f>((H20-M20)/H20)</f>
         <v>0.18400000000000008</v>
       </c>
-      <c r="S20" s="8">
+      <c r="S20" s="36">
         <f t="shared" ref="S20:S25" si="5">((I20-N20)/I20)</f>
         <v>1.801801801801807E-2</v>
       </c>
-      <c r="T20" s="8">
+      <c r="T20" s="36">
         <f t="shared" ref="T20:T25" si="6">((J20-O20)/J20)</f>
         <v>7.1428571428573005E-3</v>
       </c>
-      <c r="U20" s="9">
+      <c r="U20" s="37">
         <f t="shared" ref="U20:U25" si="7">((K20-P20)/K20)</f>
         <v>7.1428571428573005E-3</v>
       </c>
     </row>
-    <row r="21" spans="3:26" ht="24" x14ac:dyDescent="0.3">
-      <c r="C21" s="53">
+    <row r="21" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="C21" s="26">
         <v>13</v>
       </c>
-      <c r="D21" s="47" t="s">
+      <c r="D21" s="56" t="s">
         <v>27</v>
       </c>
       <c r="E21" s="2">
@@ -1861,206 +2001,206 @@
       <c r="P21" s="3">
         <v>6.9199999999999998E-8</v>
       </c>
-      <c r="Q21" s="33"/>
-      <c r="R21" s="4">
+      <c r="Q21" s="14"/>
+      <c r="R21" s="38">
         <f>((H21-M21)/H21)</f>
         <v>-2.9900332225913779E-2</v>
       </c>
-      <c r="S21" s="4">
+      <c r="S21" s="38">
         <f t="shared" ref="S21" si="8">((I21-N21)/I21)</f>
         <v>3.0188679245283012E-2</v>
       </c>
-      <c r="T21" s="4">
+      <c r="T21" s="38">
         <f t="shared" ref="T21" si="9">((J21-O21)/J21)</f>
         <v>7.3726541554959821E-2</v>
       </c>
-      <c r="U21" s="5">
+      <c r="U21" s="39">
         <f t="shared" ref="U21" si="10">((K21-P21)/K21)</f>
         <v>7.2386058981233348E-2</v>
       </c>
     </row>
-    <row r="22" spans="3:26" ht="24" x14ac:dyDescent="0.3">
-      <c r="C22" s="53">
+    <row r="22" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="C22" s="26">
         <v>14</v>
       </c>
-      <c r="D22" s="55" t="s">
+      <c r="D22" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="E22" s="32">
+      <c r="E22" s="13">
         <v>52</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22" s="4">
         <v>8502</v>
       </c>
-      <c r="G22" s="6">
+      <c r="G22" s="4">
         <v>9764</v>
       </c>
-      <c r="H22" s="7">
+      <c r="H22" s="5">
         <v>1.7300000000000001E-11</v>
       </c>
-      <c r="I22" s="7">
+      <c r="I22" s="5">
         <v>1.27E-11</v>
       </c>
-      <c r="J22" s="7">
+      <c r="J22" s="5">
         <v>4.3499999999999999E-8</v>
       </c>
-      <c r="K22" s="7">
+      <c r="K22" s="5">
         <v>4.36E-8</v>
       </c>
-      <c r="L22" s="32"/>
-      <c r="M22" s="7">
+      <c r="L22" s="13"/>
+      <c r="M22" s="5">
         <v>1.58E-11</v>
       </c>
-      <c r="N22" s="7">
+      <c r="N22" s="5">
         <v>1.1600000000000001E-11</v>
       </c>
-      <c r="O22" s="7">
+      <c r="O22" s="5">
         <v>4.1899999999999998E-8</v>
       </c>
-      <c r="P22" s="7">
+      <c r="P22" s="5">
         <v>4.1899999999999998E-8</v>
       </c>
-      <c r="Q22" s="32"/>
-      <c r="R22" s="8">
+      <c r="Q22" s="13"/>
+      <c r="R22" s="36">
         <f t="shared" ref="R22" si="11">((H22-M22)/H22)</f>
         <v>8.6705202312138796E-2</v>
       </c>
-      <c r="S22" s="8">
+      <c r="S22" s="36">
         <f t="shared" ref="S22" si="12">((I22-N22)/I22)</f>
         <v>8.6614173228346428E-2</v>
       </c>
-      <c r="T22" s="8">
+      <c r="T22" s="36">
         <f t="shared" ref="T22" si="13">((J22-O22)/J22)</f>
         <v>3.6781609195402326E-2</v>
       </c>
-      <c r="U22" s="9">
+      <c r="U22" s="37">
         <f t="shared" ref="U22" si="14">((K22-P22)/K22)</f>
         <v>3.8990825688073438E-2</v>
       </c>
     </row>
-    <row r="23" spans="3:26" ht="24" x14ac:dyDescent="0.3">
-      <c r="C23" s="53">
+    <row r="23" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="C23" s="26">
         <v>15</v>
       </c>
-      <c r="D23" s="47" t="s">
+      <c r="D23" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="E23" s="33">
+      <c r="E23" s="14">
         <v>24</v>
       </c>
-      <c r="F23" s="33">
+      <c r="F23" s="14">
         <v>10913</v>
       </c>
-      <c r="G23" s="33">
+      <c r="G23" s="14">
         <v>9955</v>
       </c>
-      <c r="H23" s="35">
+      <c r="H23" s="16">
         <v>5.1600000000000001E-11</v>
       </c>
-      <c r="I23" s="35">
+      <c r="I23" s="16">
         <v>3.0600000000000003E-11</v>
       </c>
-      <c r="J23" s="35">
+      <c r="J23" s="16">
         <v>4.4899999999999998E-8</v>
       </c>
-      <c r="K23" s="35">
+      <c r="K23" s="16">
         <v>4.4999999999999999E-8</v>
       </c>
-      <c r="L23" s="33"/>
-      <c r="M23" s="35">
+      <c r="L23" s="14"/>
+      <c r="M23" s="16">
         <v>4.8999999999999999E-11</v>
       </c>
-      <c r="N23" s="35">
+      <c r="N23" s="16">
         <v>2.2600000000000001E-11</v>
       </c>
-      <c r="O23" s="35">
+      <c r="O23" s="16">
         <v>4.5900000000000001E-8</v>
       </c>
-      <c r="P23" s="35">
+      <c r="P23" s="16">
         <v>4.6000000000000002E-8</v>
       </c>
-      <c r="Q23" s="36"/>
-      <c r="R23" s="37">
+      <c r="Q23" s="17"/>
+      <c r="R23" s="40">
         <f t="shared" ref="R23" si="15">((H23-M23)/H23)</f>
         <v>5.0387596899224854E-2</v>
       </c>
-      <c r="S23" s="37">
+      <c r="S23" s="40">
         <f t="shared" ref="S23" si="16">((I23-N23)/I23)</f>
         <v>0.26143790849673204</v>
       </c>
-      <c r="T23" s="37">
+      <c r="T23" s="40">
         <f t="shared" ref="T23" si="17">((J23-O23)/J23)</f>
         <v>-2.227171492204905E-2</v>
       </c>
-      <c r="U23" s="49">
+      <c r="U23" s="41">
         <f t="shared" ref="U23" si="18">((K23-P23)/K23)</f>
         <v>-2.2222222222222275E-2</v>
       </c>
     </row>
-    <row r="24" spans="3:26" ht="24" x14ac:dyDescent="0.3">
-      <c r="C24" s="53">
+    <row r="24" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="C24" s="26">
         <v>16</v>
       </c>
-      <c r="D24" s="55" t="s">
+      <c r="D24" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="E24" s="32">
+      <c r="E24" s="13">
         <v>258</v>
       </c>
-      <c r="F24" s="32">
+      <c r="F24" s="13">
         <v>12465</v>
       </c>
-      <c r="G24" s="32">
+      <c r="G24" s="13">
         <v>8739</v>
       </c>
-      <c r="H24" s="38">
+      <c r="H24" s="18">
         <v>4.4400000000000002E-10</v>
       </c>
-      <c r="I24" s="38">
+      <c r="I24" s="18">
         <v>3.2700000000000001E-10</v>
       </c>
-      <c r="J24" s="38">
+      <c r="J24" s="18">
         <v>2.1E-7</v>
       </c>
-      <c r="K24" s="38">
+      <c r="K24" s="18">
         <v>2.1E-7</v>
       </c>
-      <c r="L24" s="32"/>
-      <c r="M24" s="38">
+      <c r="L24" s="13"/>
+      <c r="M24" s="18">
         <v>3.9E-10</v>
       </c>
-      <c r="N24" s="38">
+      <c r="N24" s="18">
         <v>2.5100000000000001E-10</v>
       </c>
-      <c r="O24" s="38">
+      <c r="O24" s="18">
         <v>2.0200000000000001E-7</v>
       </c>
-      <c r="P24" s="38">
+      <c r="P24" s="18">
         <v>2.03E-7</v>
       </c>
-      <c r="Q24" s="32"/>
-      <c r="R24" s="8">
+      <c r="Q24" s="13"/>
+      <c r="R24" s="36">
         <f t="shared" ref="R24" si="19">((H24-M24)/H24)</f>
         <v>0.12162162162162166</v>
       </c>
-      <c r="S24" s="8">
+      <c r="S24" s="36">
         <f t="shared" ref="S24" si="20">((I24-N24)/I24)</f>
         <v>0.23241590214067276</v>
       </c>
-      <c r="T24" s="8">
+      <c r="T24" s="36">
         <f t="shared" ref="T24" si="21">((J24-O24)/J24)</f>
         <v>3.8095238095238057E-2</v>
       </c>
-      <c r="U24" s="9">
+      <c r="U24" s="37">
         <f t="shared" ref="U24" si="22">((K24-P24)/K24)</f>
         <v>3.3333333333333319E-2</v>
       </c>
     </row>
-    <row r="25" spans="3:26" ht="24" x14ac:dyDescent="0.3">
-      <c r="C25" s="53">
+    <row r="25" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="C25" s="26">
         <v>17</v>
       </c>
-      <c r="D25" s="47" t="s">
+      <c r="D25" s="56" t="s">
         <v>25</v>
       </c>
       <c r="E25" s="2">
@@ -2097,298 +2237,1369 @@
       <c r="P25" s="3">
         <v>1.3300000000000001E-7</v>
       </c>
-      <c r="Q25" s="33"/>
-      <c r="R25" s="4">
+      <c r="Q25" s="14"/>
+      <c r="R25" s="38">
         <f t="shared" ref="R25" si="23">((H25-M25)/H25)</f>
         <v>-1.0765957446808512</v>
       </c>
-      <c r="S25" s="4">
+      <c r="S25" s="38">
         <f t="shared" si="5"/>
         <v>5.9523809523809833E-3</v>
       </c>
-      <c r="T25" s="4">
+      <c r="T25" s="38">
         <f t="shared" si="6"/>
         <v>-8.1300813008130163E-2</v>
       </c>
-      <c r="U25" s="5">
+      <c r="U25" s="39">
         <f t="shared" si="7"/>
         <v>-8.1300813008130163E-2</v>
       </c>
     </row>
-    <row r="26" spans="3:26" ht="24" x14ac:dyDescent="0.3">
-      <c r="C26" s="53">
+    <row r="26" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="C26" s="26">
         <v>18</v>
       </c>
-      <c r="D26" s="55" t="s">
+      <c r="D26" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="E26" s="32">
+      <c r="E26" s="13">
         <v>3</v>
       </c>
-      <c r="F26" s="32">
+      <c r="F26" s="13">
         <v>2457</v>
       </c>
-      <c r="G26" s="32">
+      <c r="G26" s="13">
         <v>2330</v>
       </c>
-      <c r="H26" s="38">
+      <c r="H26" s="18">
         <v>1.7700000000000001E-11</v>
       </c>
-      <c r="I26" s="38">
+      <c r="I26" s="18">
         <v>1.42E-11</v>
       </c>
-      <c r="J26" s="38">
+      <c r="J26" s="18">
         <v>2.6499999999999999E-8</v>
       </c>
-      <c r="K26" s="38">
+      <c r="K26" s="18">
         <v>2.6499999999999999E-8</v>
       </c>
-      <c r="L26" s="32"/>
-      <c r="M26" s="38">
+      <c r="L26" s="13"/>
+      <c r="M26" s="18">
         <v>1.0399999999999999E-11</v>
       </c>
-      <c r="N26" s="38">
+      <c r="N26" s="18">
         <v>1.44E-11</v>
       </c>
-      <c r="O26" s="38">
+      <c r="O26" s="18">
         <v>2.6000000000000001E-8</v>
       </c>
-      <c r="P26" s="38">
+      <c r="P26" s="18">
         <v>2.6000000000000001E-8</v>
       </c>
-      <c r="Q26" s="32"/>
-      <c r="R26" s="8">
+      <c r="Q26" s="13"/>
+      <c r="R26" s="36">
         <f t="shared" ref="R26" si="24">((H26-M26)/H26)</f>
         <v>0.41242937853107353</v>
       </c>
-      <c r="S26" s="8">
+      <c r="S26" s="36">
         <f t="shared" ref="S26" si="25">((I26-N26)/I26)</f>
         <v>-1.4084507042253518E-2</v>
       </c>
-      <c r="T26" s="8">
+      <c r="T26" s="36">
         <f t="shared" ref="T26" si="26">((J26-O26)/J26)</f>
         <v>1.8867924528301806E-2</v>
       </c>
-      <c r="U26" s="9">
+      <c r="U26" s="37">
         <f t="shared" ref="U26" si="27">((K26-P26)/K26)</f>
         <v>1.8867924528301806E-2</v>
       </c>
     </row>
-    <row r="27" spans="3:26" ht="24" x14ac:dyDescent="0.3">
-      <c r="C27" s="53">
+    <row r="27" spans="3:26" x14ac:dyDescent="0.3">
+      <c r="C27" s="26">
         <v>19</v>
       </c>
-      <c r="D27" s="47" t="s">
+      <c r="D27" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="E27" s="33">
+      <c r="E27" s="14">
         <v>74</v>
       </c>
-      <c r="F27" s="33">
+      <c r="F27" s="14">
         <v>19728</v>
       </c>
-      <c r="G27" s="33">
+      <c r="G27" s="14">
         <v>17133</v>
       </c>
-      <c r="H27" s="35">
+      <c r="H27" s="16">
         <v>2.1999999999999999E-10</v>
       </c>
-      <c r="I27" s="35">
+      <c r="I27" s="16">
         <v>1.81E-10</v>
       </c>
-      <c r="J27" s="35">
+      <c r="J27" s="16">
         <v>7.4700000000000001E-8</v>
       </c>
-      <c r="K27" s="35">
+      <c r="K27" s="16">
         <v>7.5100000000000004E-8</v>
       </c>
-      <c r="L27" s="33"/>
-      <c r="M27" s="35">
+      <c r="L27" s="14"/>
+      <c r="M27" s="16">
         <v>2.4199999999999999E-10</v>
       </c>
-      <c r="N27" s="35">
+      <c r="N27" s="16">
         <v>1.5500000000000001E-10</v>
       </c>
-      <c r="O27" s="35">
+      <c r="O27" s="16">
         <v>6.4799999999999998E-8</v>
       </c>
-      <c r="P27" s="35">
+      <c r="P27" s="16">
         <v>6.5099999999999994E-8</v>
       </c>
-      <c r="Q27" s="36"/>
-      <c r="R27" s="37">
+      <c r="Q27" s="17"/>
+      <c r="R27" s="40">
         <f t="shared" ref="R27:R28" si="28">((H27-M27)/H27)</f>
         <v>-0.1</v>
       </c>
-      <c r="S27" s="37">
+      <c r="S27" s="40">
         <f t="shared" ref="S27:S28" si="29">((I27-N27)/I27)</f>
         <v>0.14364640883977894</v>
       </c>
-      <c r="T27" s="37">
+      <c r="T27" s="40">
         <f t="shared" ref="T27:T28" si="30">((J27-O27)/J27)</f>
         <v>0.13253012048192775</v>
       </c>
-      <c r="U27" s="49">
+      <c r="U27" s="41">
         <f t="shared" ref="U27:U28" si="31">((K27-P27)/K27)</f>
         <v>0.13315579227696417</v>
       </c>
     </row>
-    <row r="28" spans="3:26" ht="25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C28" s="53">
+    <row r="28" spans="3:26" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C28" s="26">
         <v>20</v>
       </c>
-      <c r="D28" s="56" t="s">
+      <c r="D28" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="E28" s="50">
+      <c r="E28" s="23">
         <v>99</v>
       </c>
-      <c r="F28" s="50">
+      <c r="F28" s="23">
         <v>11040</v>
       </c>
-      <c r="G28" s="50">
+      <c r="G28" s="23">
         <v>10525</v>
       </c>
-      <c r="H28" s="51">
+      <c r="H28" s="24">
         <v>6.3800000000000002E-11</v>
       </c>
-      <c r="I28" s="51">
+      <c r="I28" s="24">
         <v>5.1200000000000002E-11</v>
       </c>
-      <c r="J28" s="51">
+      <c r="J28" s="24">
         <v>3.1599999999999998E-8</v>
       </c>
-      <c r="K28" s="51">
+      <c r="K28" s="24">
         <v>3.1699999999999999E-8</v>
       </c>
-      <c r="L28" s="50"/>
-      <c r="M28" s="51">
+      <c r="L28" s="23"/>
+      <c r="M28" s="24">
         <v>4.8299999999999997E-11</v>
       </c>
-      <c r="N28" s="51">
+      <c r="N28" s="24">
         <v>4.2100000000000002E-11</v>
       </c>
-      <c r="O28" s="51">
+      <c r="O28" s="24">
         <v>3.0799999999999998E-8</v>
       </c>
-      <c r="P28" s="51">
+      <c r="P28" s="24">
         <v>3.0899999999999999E-8</v>
       </c>
-      <c r="Q28" s="50"/>
-      <c r="R28" s="18">
+      <c r="Q28" s="23"/>
+      <c r="R28" s="42">
         <f t="shared" si="28"/>
         <v>0.24294670846394992</v>
       </c>
-      <c r="S28" s="18">
+      <c r="S28" s="42">
         <f t="shared" si="29"/>
         <v>0.177734375</v>
       </c>
-      <c r="T28" s="18">
+      <c r="T28" s="42">
         <f t="shared" si="30"/>
         <v>2.5316455696202549E-2</v>
       </c>
-      <c r="U28" s="19">
+      <c r="U28" s="43">
         <f t="shared" si="31"/>
         <v>2.5236593059936925E-2</v>
       </c>
     </row>
-    <row r="29" spans="3:26" ht="25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C29" s="54">
+    <row r="29" spans="3:26" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C29" s="27">
         <v>21</v>
       </c>
-      <c r="D29" s="57" t="s">
+      <c r="D29" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="E29" s="58">
+      <c r="E29" s="28">
         <v>53</v>
       </c>
-      <c r="F29" s="58">
+      <c r="F29" s="28">
         <v>8539</v>
       </c>
-      <c r="G29" s="58">
+      <c r="G29" s="28">
         <v>8186</v>
       </c>
-      <c r="H29" s="59">
+      <c r="H29" s="29">
         <v>1.0799999999999999E-11</v>
       </c>
-      <c r="I29" s="59">
+      <c r="I29" s="29">
         <v>7.8799999999999995E-12</v>
       </c>
-      <c r="J29" s="59">
+      <c r="J29" s="29">
         <v>2.9999999999999997E-8</v>
       </c>
-      <c r="K29" s="59">
+      <c r="K29" s="29">
         <v>2.9999999999999997E-8</v>
       </c>
-      <c r="L29" s="58"/>
-      <c r="M29" s="59">
+      <c r="L29" s="28"/>
+      <c r="M29" s="29">
         <v>1.0499999999999999E-11</v>
       </c>
-      <c r="N29" s="59">
+      <c r="N29" s="29">
         <v>7.1299999999999997E-12</v>
       </c>
-      <c r="O29" s="59">
+      <c r="O29" s="29">
         <v>2.8600000000000001E-8</v>
       </c>
-      <c r="P29" s="59">
+      <c r="P29" s="29">
         <v>2.8600000000000001E-8</v>
       </c>
-      <c r="Q29" s="58"/>
-      <c r="R29" s="18">
+      <c r="Q29" s="28"/>
+      <c r="R29" s="42">
         <f t="shared" ref="R29" si="32">((H29-M29)/H29)</f>
         <v>2.7777777777777773E-2</v>
       </c>
-      <c r="S29" s="18">
+      <c r="S29" s="42">
         <f t="shared" ref="S29" si="33">((I29-N29)/I29)</f>
         <v>9.5177664974619269E-2</v>
       </c>
-      <c r="T29" s="18">
+      <c r="T29" s="42">
         <f t="shared" ref="T29" si="34">((J29-O29)/J29)</f>
         <v>4.6666666666666537E-2</v>
       </c>
-      <c r="U29" s="19">
+      <c r="U29" s="43">
         <f t="shared" ref="U29" si="35">((K29-P29)/K29)</f>
         <v>4.6666666666666537E-2</v>
       </c>
     </row>
-    <row r="30" spans="3:26" ht="24" x14ac:dyDescent="0.3">
-      <c r="D30" s="1"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
-      <c r="Q30" s="13" t="s">
+    <row r="30" spans="3:26" ht="31" x14ac:dyDescent="0.35">
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="Q30" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="R30" s="14">
+      <c r="R30" s="44">
         <f>AVERAGE(R9:R25)</f>
         <v>0.11317020462191031</v>
       </c>
-      <c r="S30" s="14">
+      <c r="S30" s="44">
         <f>AVERAGE(S9:S25)</f>
         <v>0.24477328909469745</v>
       </c>
-      <c r="T30" s="14">
+      <c r="T30" s="44">
         <f>AVERAGE(T9:T25)</f>
         <v>9.4670627364879439E-2</v>
       </c>
-      <c r="U30" s="14">
+      <c r="U30" s="44">
         <f>AVERAGE(U9:U28)</f>
         <v>8.885214449439259E-2</v>
       </c>
     </row>
-    <row r="32" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="32" spans="3:26" x14ac:dyDescent="0.3">
       <c r="Z32" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="D33" s="16"/>
-    </row>
-    <row r="42" spans="4:9" x14ac:dyDescent="0.2">
-      <c r="I42" s="15" t="s">
+    <row r="33" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D33" s="61"/>
+    </row>
+    <row r="42" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="I42" s="9" t="s">
         <v>23</v>
       </c>
+    </row>
+    <row r="52" spans="4:17" ht="27" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="53" spans="4:17" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D53" s="85" t="s">
+        <v>35</v>
+      </c>
+      <c r="E53" s="86" t="s">
+        <v>36</v>
+      </c>
+      <c r="F53" s="63" t="s">
+        <v>37</v>
+      </c>
+      <c r="G53" s="63" t="s">
+        <v>39</v>
+      </c>
+      <c r="H53" s="63" t="s">
+        <v>38</v>
+      </c>
+      <c r="I53" s="63" t="s">
+        <v>40</v>
+      </c>
+      <c r="J53" s="63" t="s">
+        <v>41</v>
+      </c>
+      <c r="K53" s="63" t="s">
+        <v>42</v>
+      </c>
+      <c r="L53" s="63" t="s">
+        <v>43</v>
+      </c>
+      <c r="M53" s="63" t="s">
+        <v>44</v>
+      </c>
+      <c r="N53" s="63" t="s">
+        <v>45</v>
+      </c>
+      <c r="O53" s="63" t="s">
+        <v>46</v>
+      </c>
+      <c r="P53" s="67" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q53" s="87" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="54" spans="4:17" x14ac:dyDescent="0.3">
+      <c r="D54" s="77" t="s">
+        <v>49</v>
+      </c>
+      <c r="E54" s="49">
+        <v>0</v>
+      </c>
+      <c r="F54" s="50">
+        <v>3539</v>
+      </c>
+      <c r="G54" s="50">
+        <v>3539</v>
+      </c>
+      <c r="H54" s="74">
+        <v>0</v>
+      </c>
+      <c r="I54" s="50">
+        <v>4</v>
+      </c>
+      <c r="J54" s="50">
+        <v>3</v>
+      </c>
+      <c r="K54" s="50">
+        <v>0</v>
+      </c>
+      <c r="L54" s="50">
+        <v>1</v>
+      </c>
+      <c r="M54" s="50">
+        <v>4</v>
+      </c>
+      <c r="N54" s="50">
+        <v>3</v>
+      </c>
+      <c r="O54" s="50">
+        <v>0</v>
+      </c>
+      <c r="P54" s="50">
+        <v>1</v>
+      </c>
+      <c r="Q54" s="71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="4:17" x14ac:dyDescent="0.3">
+      <c r="D55" s="80" t="s">
+        <v>29</v>
+      </c>
+      <c r="E55" s="81">
+        <v>24</v>
+      </c>
+      <c r="F55" s="82">
+        <v>10913</v>
+      </c>
+      <c r="G55" s="82">
+        <v>9955</v>
+      </c>
+      <c r="H55" s="83">
+        <v>-958</v>
+      </c>
+      <c r="I55" s="82">
+        <v>25</v>
+      </c>
+      <c r="J55" s="82">
+        <v>321</v>
+      </c>
+      <c r="K55" s="82">
+        <v>803</v>
+      </c>
+      <c r="L55" s="82">
+        <v>1357</v>
+      </c>
+      <c r="M55" s="82">
+        <v>20</v>
+      </c>
+      <c r="N55" s="82">
+        <v>559</v>
+      </c>
+      <c r="O55" s="82">
+        <v>385</v>
+      </c>
+      <c r="P55" s="82">
+        <v>324</v>
+      </c>
+      <c r="Q55" s="84">
+        <v>-1218</v>
+      </c>
+    </row>
+    <row r="56" spans="4:17" x14ac:dyDescent="0.3">
+      <c r="D56" s="78" t="s">
+        <v>26</v>
+      </c>
+      <c r="E56" s="51">
+        <v>26</v>
+      </c>
+      <c r="F56" s="47">
+        <v>10501</v>
+      </c>
+      <c r="G56" s="47">
+        <v>9750</v>
+      </c>
+      <c r="H56" s="75">
+        <v>-751</v>
+      </c>
+      <c r="I56" s="47">
+        <v>43</v>
+      </c>
+      <c r="J56" s="47">
+        <v>821</v>
+      </c>
+      <c r="K56" s="47">
+        <v>1269</v>
+      </c>
+      <c r="L56" s="47">
+        <v>852</v>
+      </c>
+      <c r="M56" s="47">
+        <v>31</v>
+      </c>
+      <c r="N56" s="47">
+        <v>598</v>
+      </c>
+      <c r="O56" s="47">
+        <v>858</v>
+      </c>
+      <c r="P56" s="47">
+        <v>132</v>
+      </c>
+      <c r="Q56" s="72">
+        <v>-1366</v>
+      </c>
+    </row>
+    <row r="57" spans="4:17" x14ac:dyDescent="0.3">
+      <c r="D57" s="80" t="s">
+        <v>25</v>
+      </c>
+      <c r="E57" s="81">
+        <v>2048</v>
+      </c>
+      <c r="F57" s="82">
+        <v>41059</v>
+      </c>
+      <c r="G57" s="82">
+        <v>44881</v>
+      </c>
+      <c r="H57" s="83">
+        <v>3822</v>
+      </c>
+      <c r="I57" s="82">
+        <v>375</v>
+      </c>
+      <c r="J57" s="82">
+        <v>2139</v>
+      </c>
+      <c r="K57" s="82">
+        <v>37</v>
+      </c>
+      <c r="L57" s="82">
+        <v>1486</v>
+      </c>
+      <c r="M57" s="82">
+        <v>220</v>
+      </c>
+      <c r="N57" s="82">
+        <v>2635</v>
+      </c>
+      <c r="O57" s="82">
+        <v>84</v>
+      </c>
+      <c r="P57" s="82">
+        <v>421</v>
+      </c>
+      <c r="Q57" s="84">
+        <v>-677</v>
+      </c>
+    </row>
+    <row r="58" spans="4:17" x14ac:dyDescent="0.3">
+      <c r="D58" s="78" t="s">
+        <v>27</v>
+      </c>
+      <c r="E58" s="51">
+        <v>28</v>
+      </c>
+      <c r="F58" s="47">
+        <v>8800</v>
+      </c>
+      <c r="G58" s="47">
+        <v>7590</v>
+      </c>
+      <c r="H58" s="75">
+        <v>-1210</v>
+      </c>
+      <c r="I58" s="47">
+        <v>5</v>
+      </c>
+      <c r="J58" s="47">
+        <v>1136</v>
+      </c>
+      <c r="K58" s="47">
+        <v>0</v>
+      </c>
+      <c r="L58" s="47">
+        <v>206</v>
+      </c>
+      <c r="M58" s="47">
+        <v>20</v>
+      </c>
+      <c r="N58" s="47">
+        <v>141</v>
+      </c>
+      <c r="O58" s="47">
+        <v>0</v>
+      </c>
+      <c r="P58" s="47">
+        <v>162</v>
+      </c>
+      <c r="Q58" s="72">
+        <v>-1024</v>
+      </c>
+    </row>
+    <row r="59" spans="4:17" x14ac:dyDescent="0.3">
+      <c r="D59" s="80" t="s">
+        <v>10</v>
+      </c>
+      <c r="E59" s="81">
+        <v>24</v>
+      </c>
+      <c r="F59" s="82">
+        <v>4110</v>
+      </c>
+      <c r="G59" s="82">
+        <v>3756</v>
+      </c>
+      <c r="H59" s="83">
+        <v>-354</v>
+      </c>
+      <c r="I59" s="82">
+        <v>4</v>
+      </c>
+      <c r="J59" s="82">
+        <v>180</v>
+      </c>
+      <c r="K59" s="82">
+        <v>50</v>
+      </c>
+      <c r="L59" s="82">
+        <v>35</v>
+      </c>
+      <c r="M59" s="82">
+        <v>5</v>
+      </c>
+      <c r="N59" s="82">
+        <v>178</v>
+      </c>
+      <c r="O59" s="82">
+        <v>22</v>
+      </c>
+      <c r="P59" s="82">
+        <v>23</v>
+      </c>
+      <c r="Q59" s="84">
+        <v>-41</v>
+      </c>
+    </row>
+    <row r="60" spans="4:17" x14ac:dyDescent="0.3">
+      <c r="D60" s="78" t="s">
+        <v>50</v>
+      </c>
+      <c r="E60" s="51">
+        <v>55</v>
+      </c>
+      <c r="F60" s="47">
+        <v>9104</v>
+      </c>
+      <c r="G60" s="47">
+        <v>9016</v>
+      </c>
+      <c r="H60" s="75">
+        <v>-88</v>
+      </c>
+      <c r="I60" s="47">
+        <v>3</v>
+      </c>
+      <c r="J60" s="47">
+        <v>887</v>
+      </c>
+      <c r="K60" s="47">
+        <v>47</v>
+      </c>
+      <c r="L60" s="47">
+        <v>587</v>
+      </c>
+      <c r="M60" s="47">
+        <v>2</v>
+      </c>
+      <c r="N60" s="47">
+        <v>884</v>
+      </c>
+      <c r="O60" s="47">
+        <v>30</v>
+      </c>
+      <c r="P60" s="47">
+        <v>768</v>
+      </c>
+      <c r="Q60" s="72">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="61" spans="4:17" x14ac:dyDescent="0.3">
+      <c r="D61" s="80" t="s">
+        <v>51</v>
+      </c>
+      <c r="E61" s="81">
+        <v>0</v>
+      </c>
+      <c r="F61" s="82">
+        <v>3980</v>
+      </c>
+      <c r="G61" s="82">
+        <v>3987</v>
+      </c>
+      <c r="H61" s="83">
+        <v>7</v>
+      </c>
+      <c r="I61" s="82">
+        <v>10</v>
+      </c>
+      <c r="J61" s="82">
+        <v>8</v>
+      </c>
+      <c r="K61" s="82">
+        <v>3</v>
+      </c>
+      <c r="L61" s="82">
+        <v>21</v>
+      </c>
+      <c r="M61" s="82">
+        <v>9</v>
+      </c>
+      <c r="N61" s="82">
+        <v>7</v>
+      </c>
+      <c r="O61" s="82">
+        <v>3</v>
+      </c>
+      <c r="P61" s="82">
+        <v>22</v>
+      </c>
+      <c r="Q61" s="84">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="62" spans="4:17" x14ac:dyDescent="0.3">
+      <c r="D62" s="78" t="s">
+        <v>52</v>
+      </c>
+      <c r="E62" s="51">
+        <v>0</v>
+      </c>
+      <c r="F62" s="47">
+        <v>881</v>
+      </c>
+      <c r="G62" s="47">
+        <v>881</v>
+      </c>
+      <c r="H62" s="75">
+        <v>0</v>
+      </c>
+      <c r="I62" s="47">
+        <v>7</v>
+      </c>
+      <c r="J62" s="47">
+        <v>100</v>
+      </c>
+      <c r="K62" s="47">
+        <v>0</v>
+      </c>
+      <c r="L62" s="47">
+        <v>8</v>
+      </c>
+      <c r="M62" s="47">
+        <v>7</v>
+      </c>
+      <c r="N62" s="47">
+        <v>100</v>
+      </c>
+      <c r="O62" s="47">
+        <v>0</v>
+      </c>
+      <c r="P62" s="47">
+        <v>8</v>
+      </c>
+      <c r="Q62" s="72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="4:17" x14ac:dyDescent="0.3">
+      <c r="D63" s="80" t="s">
+        <v>8</v>
+      </c>
+      <c r="E63" s="81">
+        <v>8</v>
+      </c>
+      <c r="F63" s="82">
+        <v>295</v>
+      </c>
+      <c r="G63" s="82">
+        <v>297</v>
+      </c>
+      <c r="H63" s="83">
+        <v>2</v>
+      </c>
+      <c r="I63" s="82">
+        <v>0</v>
+      </c>
+      <c r="J63" s="82">
+        <v>10</v>
+      </c>
+      <c r="K63" s="82">
+        <v>0</v>
+      </c>
+      <c r="L63" s="82">
+        <v>0</v>
+      </c>
+      <c r="M63" s="82">
+        <v>1</v>
+      </c>
+      <c r="N63" s="82">
+        <v>2</v>
+      </c>
+      <c r="O63" s="82">
+        <v>0</v>
+      </c>
+      <c r="P63" s="82">
+        <v>0</v>
+      </c>
+      <c r="Q63" s="84">
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="64" spans="4:17" x14ac:dyDescent="0.3">
+      <c r="D64" s="78" t="s">
+        <v>6</v>
+      </c>
+      <c r="E64" s="51">
+        <v>110</v>
+      </c>
+      <c r="F64" s="47">
+        <v>1435</v>
+      </c>
+      <c r="G64" s="47">
+        <v>1162</v>
+      </c>
+      <c r="H64" s="75">
+        <v>-273</v>
+      </c>
+      <c r="I64" s="47">
+        <v>15</v>
+      </c>
+      <c r="J64" s="47">
+        <v>113</v>
+      </c>
+      <c r="K64" s="47">
+        <v>9</v>
+      </c>
+      <c r="L64" s="47">
+        <v>25</v>
+      </c>
+      <c r="M64" s="47">
+        <v>4</v>
+      </c>
+      <c r="N64" s="47">
+        <v>54</v>
+      </c>
+      <c r="O64" s="47">
+        <v>7</v>
+      </c>
+      <c r="P64" s="47">
+        <v>7</v>
+      </c>
+      <c r="Q64" s="72">
+        <v>-90</v>
+      </c>
+    </row>
+    <row r="65" spans="4:17" x14ac:dyDescent="0.3">
+      <c r="D65" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="E65" s="81">
+        <v>11</v>
+      </c>
+      <c r="F65" s="82">
+        <v>1954</v>
+      </c>
+      <c r="G65" s="82">
+        <v>1785</v>
+      </c>
+      <c r="H65" s="83">
+        <v>-169</v>
+      </c>
+      <c r="I65" s="82">
+        <v>13</v>
+      </c>
+      <c r="J65" s="82">
+        <v>124</v>
+      </c>
+      <c r="K65" s="82">
+        <v>10</v>
+      </c>
+      <c r="L65" s="82">
+        <v>34</v>
+      </c>
+      <c r="M65" s="82">
+        <v>9</v>
+      </c>
+      <c r="N65" s="82">
+        <v>118</v>
+      </c>
+      <c r="O65" s="82">
+        <v>4</v>
+      </c>
+      <c r="P65" s="82">
+        <v>0</v>
+      </c>
+      <c r="Q65" s="84">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="66" spans="4:17" x14ac:dyDescent="0.3">
+      <c r="D66" s="78" t="s">
+        <v>5</v>
+      </c>
+      <c r="E66" s="51">
+        <v>450</v>
+      </c>
+      <c r="F66" s="47">
+        <v>11106</v>
+      </c>
+      <c r="G66" s="47">
+        <v>8707</v>
+      </c>
+      <c r="H66" s="75">
+        <v>-2399</v>
+      </c>
+      <c r="I66" s="47">
+        <v>292</v>
+      </c>
+      <c r="J66" s="47">
+        <v>1800</v>
+      </c>
+      <c r="K66" s="47">
+        <v>229</v>
+      </c>
+      <c r="L66" s="47">
+        <v>1272</v>
+      </c>
+      <c r="M66" s="47">
+        <v>16</v>
+      </c>
+      <c r="N66" s="47">
+        <v>332</v>
+      </c>
+      <c r="O66" s="47">
+        <v>752</v>
+      </c>
+      <c r="P66" s="47">
+        <v>15</v>
+      </c>
+      <c r="Q66" s="72">
+        <v>-2478</v>
+      </c>
+    </row>
+    <row r="67" spans="4:17" x14ac:dyDescent="0.3">
+      <c r="D67" s="80" t="s">
+        <v>4</v>
+      </c>
+      <c r="E67" s="81">
+        <v>256</v>
+      </c>
+      <c r="F67" s="82">
+        <v>8281</v>
+      </c>
+      <c r="G67" s="82">
+        <v>5722</v>
+      </c>
+      <c r="H67" s="83">
+        <v>-2559</v>
+      </c>
+      <c r="I67" s="82">
+        <v>0</v>
+      </c>
+      <c r="J67" s="82">
+        <v>0</v>
+      </c>
+      <c r="K67" s="82">
+        <v>0</v>
+      </c>
+      <c r="L67" s="82">
+        <v>0</v>
+      </c>
+      <c r="M67" s="82">
+        <v>0</v>
+      </c>
+      <c r="N67" s="82">
+        <v>0</v>
+      </c>
+      <c r="O67" s="82">
+        <v>0</v>
+      </c>
+      <c r="P67" s="82">
+        <v>0</v>
+      </c>
+      <c r="Q67" s="84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="4:17" x14ac:dyDescent="0.3">
+      <c r="D68" s="78" t="s">
+        <v>3</v>
+      </c>
+      <c r="E68" s="51">
+        <v>65</v>
+      </c>
+      <c r="F68" s="47">
+        <v>3807</v>
+      </c>
+      <c r="G68" s="47">
+        <v>1591</v>
+      </c>
+      <c r="H68" s="75">
+        <v>-2216</v>
+      </c>
+      <c r="I68" s="47">
+        <v>0</v>
+      </c>
+      <c r="J68" s="47">
+        <v>0</v>
+      </c>
+      <c r="K68" s="47">
+        <v>0</v>
+      </c>
+      <c r="L68" s="47">
+        <v>0</v>
+      </c>
+      <c r="M68" s="47">
+        <v>0</v>
+      </c>
+      <c r="N68" s="47">
+        <v>0</v>
+      </c>
+      <c r="O68" s="47">
+        <v>0</v>
+      </c>
+      <c r="P68" s="47">
+        <v>0</v>
+      </c>
+      <c r="Q68" s="72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="4:17" x14ac:dyDescent="0.3">
+      <c r="D69" s="80" t="s">
+        <v>2</v>
+      </c>
+      <c r="E69" s="81">
+        <v>9</v>
+      </c>
+      <c r="F69" s="82">
+        <v>918</v>
+      </c>
+      <c r="G69" s="82">
+        <v>858</v>
+      </c>
+      <c r="H69" s="83">
+        <v>-60</v>
+      </c>
+      <c r="I69" s="82">
+        <v>2</v>
+      </c>
+      <c r="J69" s="82">
+        <v>96</v>
+      </c>
+      <c r="K69" s="82">
+        <v>1</v>
+      </c>
+      <c r="L69" s="82">
+        <v>10</v>
+      </c>
+      <c r="M69" s="82">
+        <v>0</v>
+      </c>
+      <c r="N69" s="82">
+        <v>80</v>
+      </c>
+      <c r="O69" s="82">
+        <v>1</v>
+      </c>
+      <c r="P69" s="82">
+        <v>5</v>
+      </c>
+      <c r="Q69" s="84">
+        <v>-23</v>
+      </c>
+    </row>
+    <row r="70" spans="4:17" x14ac:dyDescent="0.3">
+      <c r="D70" s="78" t="s">
+        <v>24</v>
+      </c>
+      <c r="E70" s="51">
+        <v>247</v>
+      </c>
+      <c r="F70" s="47">
+        <v>96821</v>
+      </c>
+      <c r="G70" s="47">
+        <v>91114</v>
+      </c>
+      <c r="H70" s="75">
+        <v>-5707</v>
+      </c>
+      <c r="I70" s="47">
+        <v>884</v>
+      </c>
+      <c r="J70" s="47">
+        <v>9282</v>
+      </c>
+      <c r="K70" s="47">
+        <v>81</v>
+      </c>
+      <c r="L70" s="47">
+        <v>1282</v>
+      </c>
+      <c r="M70" s="47">
+        <v>161</v>
+      </c>
+      <c r="N70" s="47">
+        <v>7081</v>
+      </c>
+      <c r="O70" s="47">
+        <v>64</v>
+      </c>
+      <c r="P70" s="47">
+        <v>400</v>
+      </c>
+      <c r="Q70" s="72">
+        <v>-3823</v>
+      </c>
+    </row>
+    <row r="71" spans="4:17" x14ac:dyDescent="0.3">
+      <c r="D71" s="80" t="s">
+        <v>30</v>
+      </c>
+      <c r="E71" s="81">
+        <v>258</v>
+      </c>
+      <c r="F71" s="82">
+        <v>12465</v>
+      </c>
+      <c r="G71" s="82">
+        <v>8739</v>
+      </c>
+      <c r="H71" s="83">
+        <v>-3726</v>
+      </c>
+      <c r="I71" s="82">
+        <v>31</v>
+      </c>
+      <c r="J71" s="82">
+        <v>513</v>
+      </c>
+      <c r="K71" s="82">
+        <v>40</v>
+      </c>
+      <c r="L71" s="82">
+        <v>160</v>
+      </c>
+      <c r="M71" s="82">
+        <v>34</v>
+      </c>
+      <c r="N71" s="82">
+        <v>217</v>
+      </c>
+      <c r="O71" s="82">
+        <v>46</v>
+      </c>
+      <c r="P71" s="82">
+        <v>149</v>
+      </c>
+      <c r="Q71" s="84">
+        <v>-298</v>
+      </c>
+    </row>
+    <row r="72" spans="4:17" x14ac:dyDescent="0.3">
+      <c r="D72" s="78" t="s">
+        <v>31</v>
+      </c>
+      <c r="E72" s="51">
+        <v>3</v>
+      </c>
+      <c r="F72" s="47">
+        <v>2457</v>
+      </c>
+      <c r="G72" s="47">
+        <v>2330</v>
+      </c>
+      <c r="H72" s="75">
+        <v>-127</v>
+      </c>
+      <c r="I72" s="47">
+        <v>13</v>
+      </c>
+      <c r="J72" s="47">
+        <v>59</v>
+      </c>
+      <c r="K72" s="47">
+        <v>0</v>
+      </c>
+      <c r="L72" s="47">
+        <v>0</v>
+      </c>
+      <c r="M72" s="47">
+        <v>12</v>
+      </c>
+      <c r="N72" s="47">
+        <v>58</v>
+      </c>
+      <c r="O72" s="47">
+        <v>0</v>
+      </c>
+      <c r="P72" s="47">
+        <v>0</v>
+      </c>
+      <c r="Q72" s="72">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="73" spans="4:17" x14ac:dyDescent="0.3">
+      <c r="D73" s="80" t="s">
+        <v>32</v>
+      </c>
+      <c r="E73" s="81">
+        <v>74</v>
+      </c>
+      <c r="F73" s="82">
+        <v>19728</v>
+      </c>
+      <c r="G73" s="82">
+        <v>17133</v>
+      </c>
+      <c r="H73" s="83">
+        <v>-2595</v>
+      </c>
+      <c r="I73" s="82">
+        <v>70</v>
+      </c>
+      <c r="J73" s="82">
+        <v>1199</v>
+      </c>
+      <c r="K73" s="82">
+        <v>29</v>
+      </c>
+      <c r="L73" s="82">
+        <v>550</v>
+      </c>
+      <c r="M73" s="82">
+        <v>32</v>
+      </c>
+      <c r="N73" s="82">
+        <v>1113</v>
+      </c>
+      <c r="O73" s="82">
+        <v>1051</v>
+      </c>
+      <c r="P73" s="82">
+        <v>582</v>
+      </c>
+      <c r="Q73" s="84">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="74" spans="4:17" x14ac:dyDescent="0.3">
+      <c r="D74" s="78" t="s">
+        <v>33</v>
+      </c>
+      <c r="E74" s="51">
+        <v>102</v>
+      </c>
+      <c r="F74" s="47">
+        <v>14370</v>
+      </c>
+      <c r="G74" s="47">
+        <v>13676</v>
+      </c>
+      <c r="H74" s="75">
+        <v>-694</v>
+      </c>
+      <c r="I74" s="47">
+        <v>102</v>
+      </c>
+      <c r="J74" s="47">
+        <v>1142</v>
+      </c>
+      <c r="K74" s="47">
+        <v>22</v>
+      </c>
+      <c r="L74" s="47">
+        <v>93</v>
+      </c>
+      <c r="M74" s="47">
+        <v>146</v>
+      </c>
+      <c r="N74" s="47">
+        <v>1262</v>
+      </c>
+      <c r="O74" s="47">
+        <v>26</v>
+      </c>
+      <c r="P74" s="47">
+        <v>109</v>
+      </c>
+      <c r="Q74" s="72">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="75" spans="4:17" x14ac:dyDescent="0.3">
+      <c r="D75" s="80" t="s">
+        <v>34</v>
+      </c>
+      <c r="E75" s="81">
+        <v>53</v>
+      </c>
+      <c r="F75" s="82">
+        <v>8539</v>
+      </c>
+      <c r="G75" s="82">
+        <v>8186</v>
+      </c>
+      <c r="H75" s="83">
+        <v>-353</v>
+      </c>
+      <c r="I75" s="82">
+        <v>27</v>
+      </c>
+      <c r="J75" s="82">
+        <v>336</v>
+      </c>
+      <c r="K75" s="82">
+        <v>607</v>
+      </c>
+      <c r="L75" s="82">
+        <v>65</v>
+      </c>
+      <c r="M75" s="82">
+        <v>86</v>
+      </c>
+      <c r="N75" s="82">
+        <v>422</v>
+      </c>
+      <c r="O75" s="82">
+        <v>667</v>
+      </c>
+      <c r="P75" s="82">
+        <v>59</v>
+      </c>
+      <c r="Q75" s="84">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="76" spans="4:17" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D76" s="79" t="s">
+        <v>22</v>
+      </c>
+      <c r="E76" s="52">
+        <v>0</v>
+      </c>
+      <c r="F76" s="48">
+        <v>50905</v>
+      </c>
+      <c r="G76" s="48">
+        <v>50264</v>
+      </c>
+      <c r="H76" s="76">
+        <v>-641</v>
+      </c>
+      <c r="I76" s="48">
+        <v>611</v>
+      </c>
+      <c r="J76" s="48">
+        <v>7838</v>
+      </c>
+      <c r="K76" s="48">
+        <v>71</v>
+      </c>
+      <c r="L76" s="48">
+        <v>607</v>
+      </c>
+      <c r="M76" s="48">
+        <v>592</v>
+      </c>
+      <c r="N76" s="48">
+        <v>8296</v>
+      </c>
+      <c r="O76" s="48">
+        <v>166</v>
+      </c>
+      <c r="P76" s="48">
+        <v>683</v>
+      </c>
+      <c r="Q76" s="73">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="77" spans="4:17" x14ac:dyDescent="0.3">
+      <c r="E77" s="45"/>
+      <c r="F77" s="45"/>
+      <c r="G77" s="45"/>
+      <c r="H77" s="45"/>
+      <c r="I77" s="45"/>
+      <c r="J77" s="45"/>
+      <c r="K77" s="45"/>
+      <c r="L77" s="45"/>
+      <c r="M77" s="45"/>
+      <c r="N77" s="45"/>
+      <c r="O77" s="45"/>
+      <c r="P77" s="45"/>
+      <c r="Q77" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>